<commit_message>
Excel de requerimientos, mas info
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="127">
   <si>
     <t>Nombre</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Mantenimiento de Categorias</t>
   </si>
   <si>
-    <t>Modulo de Carrito de Compras</t>
-  </si>
-  <si>
     <t>Modulo de Pedidos</t>
   </si>
   <si>
@@ -234,12 +231,6 @@
     <t>Modulo de Ayuda en el Sistema</t>
   </si>
   <si>
-    <t>Mantenimiento de Direcciones</t>
-  </si>
-  <si>
-    <t>Modulos y Mantenimientos del sistema</t>
-  </si>
-  <si>
     <t>Mantenimiento de Sliders</t>
   </si>
   <si>
@@ -330,7 +321,88 @@
     <t>Muestra los pedidos filtrados por rango de fecha, cliente y estado, funcionalidad de cambiar el estado</t>
   </si>
   <si>
-    <t>Vista del pedido con los articulos que se solicitan</t>
+    <t>Vista del pedido con los articulos que se solicitan, cambia estado</t>
+  </si>
+  <si>
+    <t>Mantenimiento Direcciones</t>
+  </si>
+  <si>
+    <t>Maximo de 3 direcciones por usuario</t>
+  </si>
+  <si>
+    <t>Vista de las 3</t>
+  </si>
+  <si>
+    <t>Modal Crear</t>
+  </si>
+  <si>
+    <t>Modal Modificar</t>
+  </si>
+  <si>
+    <t>Modulo Carrito Compras</t>
+  </si>
+  <si>
+    <t>Mostrar Total de Articulos en el carro en Layout</t>
+  </si>
+  <si>
+    <t>Vista Con Detalle de Articulos agregados</t>
+  </si>
+  <si>
+    <t>Opcion de Cambiar Cantidad o quitar articulo</t>
+  </si>
+  <si>
+    <t>Modal Procesar que elige la direccion</t>
+  </si>
+  <si>
+    <t>Vista Con Detalle de todos los pedidos, opcion de filtrar por estado y rango de fecha (opcional)</t>
+  </si>
+  <si>
+    <t>Vista Detalle de Pedido</t>
+  </si>
+  <si>
+    <t>Modulos y Mantenimientos del Sistema</t>
+  </si>
+  <si>
+    <t>Mostrar Slider con lo que sea</t>
+  </si>
+  <si>
+    <t>Mostrar Categorias Disponibles</t>
+  </si>
+  <si>
+    <t>Mostrar Articulos Mas solicitados</t>
+  </si>
+  <si>
+    <t>Mostrar Articulos Misc</t>
+  </si>
+  <si>
+    <t>Imágenes para categorias</t>
+  </si>
+  <si>
+    <t>Vista Articulos por categoria</t>
+  </si>
+  <si>
+    <t>Vista Resultados de busqueda</t>
+  </si>
+  <si>
+    <t>Info del articulo</t>
+  </si>
+  <si>
+    <t>Opcion de agregar al carro</t>
+  </si>
+  <si>
+    <t>Opcion Crear carrito con pedido anterior</t>
+  </si>
+  <si>
+    <t>Muestra info del usuario</t>
+  </si>
+  <si>
+    <t>Vista que descarga el manual</t>
+  </si>
+  <si>
+    <t>Vista con info de la empresa</t>
+  </si>
+  <si>
+    <t>Modulo con info de contacto</t>
   </si>
 </sst>
 </file>
@@ -586,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -647,75 +719,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -724,71 +730,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H169"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,67 +1639,70 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>117</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
@@ -2118,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,663 +2210,775 @@
     <col min="5" max="5" width="31.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="31.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="23"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="23"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="23"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="23"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="39" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="23"/>
+    </row>
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="72"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="73"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="75"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="23"/>
-    </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="37"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="38"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="36"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="52"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="29"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="55"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="26"/>
+        <v>82</v>
+      </c>
+      <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="62"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="L9" s="65"/>
       <c r="M9" s="23" t="s">
-        <v>66</v>
+        <v>105</v>
+      </c>
+      <c r="O9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="23"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="23" t="s">
-        <v>67</v>
+        <v>83</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+      <c r="O10" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
+        <v>84</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
       <c r="I11" s="23"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="23" t="s">
-        <v>68</v>
+      <c r="K11" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="O11" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="45"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="56"/>
-      <c r="H12" s="57"/>
+        <v>76</v>
+      </c>
+      <c r="F12" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="64"/>
+      <c r="H12" s="65"/>
       <c r="I12" s="23"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="24"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="P12" s="27"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="26"/>
+        <v>82</v>
+      </c>
+      <c r="D13" s="24"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="59"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="23"/>
-      <c r="L13" s="26"/>
+      <c r="K13" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" s="24"/>
       <c r="M13" s="23" t="s">
-        <v>84</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="O13" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="P13" s="60"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="61"/>
+        <v>83</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="23"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="23" t="s">
-        <v>69</v>
-      </c>
+      <c r="L14" s="24"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="26"/>
+        <v>84</v>
+      </c>
+      <c r="D15" s="24"/>
       <c r="E15" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="67" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
+        <v>74</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="23"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="23" t="s">
-        <v>80</v>
-      </c>
+      <c r="L15" s="24"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="45"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="25"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="23"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="24"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="P16" s="23"/>
+    </row>
+    <row r="17" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="23"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="P17" s="27"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="F18" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="40"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="23"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="O18" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="23"/>
+      <c r="L19" s="24"/>
+      <c r="O19" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="23"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="23"/>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="26"/>
-      <c r="F18" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="71"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="23"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="23"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="23"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="70"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="23"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="23"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="24"/>
+      <c r="O20" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="23"/>
+      <c r="L21" s="24"/>
+      <c r="O21" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="23"/>
+      <c r="L22" s="24"/>
+      <c r="O22" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="P22" s="23"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="P23" s="27"/>
+    </row>
+    <row r="24" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="66" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="25"/>
+      <c r="F24" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="O24" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="P24" s="23"/>
+    </row>
+    <row r="25" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="P25" s="27"/>
+    </row>
+    <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="39"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="N26" s="30"/>
+      <c r="O26" s="80" t="s">
+        <v>123</v>
+      </c>
+      <c r="P26" s="30"/>
+    </row>
+    <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="F27" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="40"/>
+      <c r="H27" s="41"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="N27" s="30"/>
+      <c r="O27" s="80" t="s">
+        <v>124</v>
+      </c>
+      <c r="P27" s="30"/>
+    </row>
+    <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="41"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N28" s="30"/>
+      <c r="O28" s="80" t="s">
+        <v>125</v>
+      </c>
+      <c r="P28" s="30"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="24"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="41"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="O29" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D30" s="24"/>
+      <c r="F30" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="66"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="23"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="23"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="23"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="23"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="26"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="59"/>
-      <c r="L23" s="26"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
-      <c r="B24" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="45"/>
-      <c r="F24" s="66" t="s">
+      <c r="G30" s="42"/>
+      <c r="H30" s="39"/>
+      <c r="L30" s="24"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="24"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="44"/>
+      <c r="L31" s="24"/>
+    </row>
+    <row r="32" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="24"/>
+      <c r="E32" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="L32" s="24"/>
+    </row>
+    <row r="33" spans="4:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="24"/>
+      <c r="E33" t="s">
         <v>97</v>
       </c>
-      <c r="G24" s="66"/>
-      <c r="H24" s="59"/>
-      <c r="L24" s="26"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="26"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="59"/>
-      <c r="L25" s="26"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="26"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="59"/>
-      <c r="L26" s="26"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="26"/>
-      <c r="F27" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="71"/>
-      <c r="H27" s="70"/>
-      <c r="L27" s="26"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="26"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="70"/>
-      <c r="L28" s="26"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D29" s="26"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="70"/>
-      <c r="L29" s="26"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D30" s="26"/>
-      <c r="F30" s="58" t="s">
+      <c r="F33" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="G30" s="58"/>
-      <c r="H30" s="59"/>
-      <c r="L30" s="26"/>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="26"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="73"/>
-      <c r="L31" s="26"/>
-    </row>
-    <row r="32" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="26"/>
-      <c r="E32" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32" s="52" t="s">
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
+      <c r="L33" s="24"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D34" s="24"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
+      <c r="L34" s="24"/>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D35" s="24"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
+      <c r="L35" s="24"/>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D36" s="24"/>
+      <c r="F36" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="G32" s="52"/>
-      <c r="H32" s="53"/>
-      <c r="L32" s="26"/>
-    </row>
-    <row r="33" spans="4:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="26"/>
-      <c r="E33" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="74" t="s">
-        <v>101</v>
-      </c>
-      <c r="G33" s="74"/>
-      <c r="H33" s="75"/>
-      <c r="L33" s="26"/>
-    </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D34" s="26"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="77"/>
-      <c r="L34" s="26"/>
-    </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="26"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="77"/>
-      <c r="L35" s="26"/>
-    </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D36" s="26"/>
-      <c r="F36" s="66" t="s">
-        <v>102</v>
-      </c>
-      <c r="G36" s="66"/>
-      <c r="H36" s="59"/>
-      <c r="L36" s="26"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="39"/>
+      <c r="L36" s="24"/>
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D37" s="26"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="59"/>
-      <c r="L37" s="26"/>
+      <c r="D37" s="24"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="39"/>
+      <c r="L37" s="24"/>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="L38" s="26"/>
+      <c r="D38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="L38" s="24"/>
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="L39" s="26"/>
+      <c r="D39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="L39" s="24"/>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="L40" s="26"/>
+      <c r="D40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="L40" s="24"/>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="L41" s="26"/>
+      <c r="D41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="L41" s="24"/>
     </row>
     <row r="42" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="L42" s="26"/>
+      <c r="D42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="L42" s="24"/>
     </row>
     <row r="43" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="L43" s="26"/>
+      <c r="D43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="L43" s="24"/>
     </row>
     <row r="44" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="L44" s="26"/>
+      <c r="D44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="L44" s="24"/>
     </row>
     <row r="45" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="L45" s="26"/>
+      <c r="D45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="L45" s="24"/>
     </row>
     <row r="46" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="L46" s="26"/>
+      <c r="D46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="L46" s="24"/>
     </row>
     <row r="47" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="L47" s="26"/>
+      <c r="D47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="L47" s="24"/>
     </row>
     <row r="48" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="L48" s="26"/>
+      <c r="D48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="L48" s="24"/>
     </row>
     <row r="49" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="L49" s="26"/>
+      <c r="D49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="L49" s="24"/>
     </row>
     <row r="50" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="L50" s="26"/>
+      <c r="D50" s="24"/>
+      <c r="H50" s="24"/>
+      <c r="L50" s="24"/>
     </row>
     <row r="51" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="L51" s="26"/>
+      <c r="D51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="L51" s="24"/>
     </row>
     <row r="52" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="L52" s="26"/>
+      <c r="D52" s="24"/>
+      <c r="H52" s="24"/>
+      <c r="L52" s="24"/>
     </row>
     <row r="53" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="L53" s="26"/>
+      <c r="D53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="L53" s="24"/>
     </row>
     <row r="54" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D54" s="26"/>
-      <c r="H54" s="26"/>
-      <c r="L54" s="26"/>
+      <c r="D54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="L54" s="24"/>
     </row>
     <row r="55" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="L55" s="26"/>
+      <c r="D55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="L55" s="24"/>
     </row>
     <row r="56" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D56" s="26"/>
-      <c r="H56" s="26"/>
-      <c r="L56" s="26"/>
+      <c r="D56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="L56" s="24"/>
     </row>
     <row r="57" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="L57" s="26"/>
+      <c r="D57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="L57" s="24"/>
     </row>
     <row r="58" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="L58" s="26"/>
+      <c r="D58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="L58" s="24"/>
     </row>
     <row r="59" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="L59" s="26"/>
+      <c r="D59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="L59" s="24"/>
     </row>
     <row r="60" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D60" s="26"/>
-      <c r="H60" s="26"/>
-      <c r="L60" s="26"/>
+      <c r="D60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="L60" s="24"/>
     </row>
     <row r="61" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="L61" s="26"/>
+      <c r="D61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="L61" s="24"/>
     </row>
     <row r="62" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D62" s="26"/>
-      <c r="H62" s="26"/>
-      <c r="L62" s="26"/>
+      <c r="D62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="L62" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="F12:H13"/>
+    <mergeCell ref="A2:P3"/>
+    <mergeCell ref="A4:H6"/>
+    <mergeCell ref="I4:P6"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="O13:P15"/>
+    <mergeCell ref="F15:H17"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M7:P8"/>
     <mergeCell ref="F33:H35"/>
     <mergeCell ref="F36:H37"/>
     <mergeCell ref="F18:H20"/>
@@ -2792,18 +2986,6 @@
     <mergeCell ref="F24:H26"/>
     <mergeCell ref="F27:H29"/>
     <mergeCell ref="F30:H31"/>
-    <mergeCell ref="F15:H17"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="F12:H13"/>
-    <mergeCell ref="A2:P3"/>
-    <mergeCell ref="A4:H6"/>
-    <mergeCell ref="I4:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Resulevo error al sincronizar clientes
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
     <sheet name="Modulos Y Mantenimientos" sheetId="2" r:id="rId2"/>
-    <sheet name="Modulos Y Mantenimientos ESTADO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="131">
   <si>
     <t>Nombre</t>
   </si>
@@ -391,9 +390,6 @@
     <t>Opcion Crear carrito con pedido anterior</t>
   </si>
   <si>
-    <t>Muestra info del usuario</t>
-  </si>
-  <si>
     <t>Vista que descarga el manual</t>
   </si>
   <si>
@@ -413,15 +409,6 @@
   </si>
   <si>
     <t>Incluye asignacion de roles</t>
-  </si>
-  <si>
-    <t>Titulo</t>
-  </si>
-  <si>
-    <t>Imagen</t>
-  </si>
-  <si>
-    <t>Estado mostrar</t>
   </si>
   <si>
     <t>Modulo de Inicio</t>
@@ -434,7 +421,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,14 +455,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -703,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -808,17 +787,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -826,11 +794,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1007,87 +970,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1395,7 +1277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -1454,7 +1336,7 @@
       <c r="A7" s="33">
         <v>2</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1474,7 +1356,7 @@
       <c r="A8" s="33">
         <v>3</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -1494,7 +1376,7 @@
       <c r="A9" s="33">
         <v>4</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1606,7 +1488,7 @@
       <c r="A15" s="16">
         <v>10</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
@@ -1624,7 +1506,7 @@
       <c r="A16" s="33">
         <v>11</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1644,7 +1526,7 @@
       <c r="A17" s="16">
         <v>12</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="44" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1734,7 +1616,7 @@
       <c r="A22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="45" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1752,7 +1634,7 @@
       <c r="A23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="45" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1770,7 +1652,7 @@
       <c r="A24" s="16">
         <v>18</v>
       </c>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="46" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="17" t="s">
@@ -1806,7 +1688,7 @@
       <c r="A26" s="16">
         <v>20</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="46" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="17" t="s">
@@ -1824,7 +1706,7 @@
       <c r="A27" s="16">
         <v>21</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="46" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -2421,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
@@ -2438,284 +2320,284 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="100"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="88"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="103"/>
+      <c r="A3" s="89"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="91"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="110" t="s">
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="106"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="94"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="106"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="94"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="107"/>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="109"/>
+      <c r="A6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="97"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="90" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="116" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="85" t="s">
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="86"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="74"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="87"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="117"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="89"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="77"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="70"/>
+      <c r="B9" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="92" t="s">
+      <c r="F9" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="92"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="112" t="s">
+      <c r="G9" s="80"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96" t="s">
+      <c r="J9" s="84"/>
+      <c r="K9" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="97"/>
+      <c r="L9" s="85"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="69" t="s">
+      <c r="O9" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="70"/>
+      <c r="P9" s="58"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="78"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="66"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="71" t="s">
+      <c r="O10" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="72"/>
+      <c r="P10" s="60"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="72"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="67" t="s">
+      <c r="F11" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="71" t="s">
+      <c r="K11" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="72"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="71" t="s">
+      <c r="O11" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="72"/>
+      <c r="P11" s="60"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="72"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="96" t="s">
+      <c r="F12" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="96"/>
-      <c r="H12" s="97"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="85"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="71" t="s">
+      <c r="K12" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="72"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="67" t="s">
+      <c r="O12" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="68"/>
+      <c r="P12" s="56"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="78"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="66"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="71" t="s">
+      <c r="K13" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="72"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="92" t="s">
+      <c r="O13" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="93"/>
+      <c r="P13" s="81"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -2727,19 +2609,19 @@
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="32"/>
       <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="95"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="83"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2751,19 +2633,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="114" t="s">
+      <c r="F15" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="114"/>
-      <c r="H15" s="115"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="103"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="94"/>
-      <c r="P15" s="95"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="83"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -2773,19 +2655,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="31"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="80"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="68"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="61" t="s">
+      <c r="O16" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="62"/>
+      <c r="P16" s="50"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -2795,19 +2677,19 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="80"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="67" t="s">
+      <c r="O17" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="68"/>
+      <c r="P17" s="56"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2819,23 +2701,23 @@
       <c r="C18" s="36"/>
       <c r="D18" s="37"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="79" t="s">
+      <c r="F18" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="79"/>
-      <c r="H18" s="80"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="68"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="19"/>
       <c r="M18" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="65" t="s">
+      <c r="O18" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="66"/>
+      <c r="P18" s="54"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -2845,19 +2727,19 @@
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="80"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="68"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="61" t="s">
+      <c r="O19" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="62"/>
+      <c r="P19" s="50"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -2867,19 +2749,19 @@
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="80"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="68"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="61" t="s">
+      <c r="O20" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="62"/>
+      <c r="P20" s="50"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -2889,21 +2771,21 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="81" t="s">
+      <c r="F21" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="81"/>
-      <c r="H21" s="78"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="66"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="61" t="s">
+      <c r="O21" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="62"/>
+      <c r="P21" s="50"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2915,19 +2797,19 @@
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="78"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="66"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="61" t="s">
+      <c r="O22" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="62"/>
+      <c r="P22" s="50"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -2937,19 +2819,19 @@
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="78"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="66"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="63" t="s">
+      <c r="O23" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="64"/>
+      <c r="P23" s="52"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -2959,11 +2841,11 @@
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="81" t="s">
+      <c r="F24" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="81"/>
-      <c r="H24" s="78"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="66"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -2972,10 +2854,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="65" t="s">
+      <c r="O24" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="66"/>
+      <c r="P24" s="54"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -2985,19 +2867,19 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="78"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="66"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="63" t="s">
+      <c r="O25" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="64"/>
+      <c r="P25" s="52"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -3009,9 +2891,9 @@
       <c r="C26" s="36"/>
       <c r="D26" s="37"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="78"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="66"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -3020,10 +2902,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="25"/>
-      <c r="O26" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="P26" s="60"/>
+      <c r="O26" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="P26" s="48"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -3033,11 +2915,11 @@
       <c r="C27" s="38"/>
       <c r="D27" s="39"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="79" t="s">
+      <c r="F27" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="79"/>
-      <c r="H27" s="80"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="68"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -3046,10 +2928,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="59" t="s">
-        <v>123</v>
-      </c>
-      <c r="P27" s="60"/>
+      <c r="O27" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="P27" s="48"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -3059,9 +2941,9 @@
       <c r="C28" s="38"/>
       <c r="D28" s="39"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="80"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -3070,10 +2952,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="P28" s="60"/>
+      <c r="O28" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="P28" s="48"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -3083,9 +2965,9 @@
       <c r="C29" s="38"/>
       <c r="D29" s="39"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="80"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="68"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -3094,33 +2976,33 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="P29" s="60"/>
+      <c r="O29" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="P29" s="48"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="81" t="s">
+      <c r="F30" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="81"/>
-      <c r="H30" s="78"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="66"/>
       <c r="L30" s="19"/>
       <c r="M30" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="O30" s="30" t="s">
         <v>126</v>
-      </c>
-      <c r="O30" s="30" t="s">
-        <v>127</v>
       </c>
       <c r="P30" s="31"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="83"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="71"/>
       <c r="L31" s="19"/>
       <c r="O31" s="30"/>
       <c r="P31" s="31"/>
@@ -3143,45 +3025,45 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="73" t="s">
+      <c r="F33" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="73"/>
-      <c r="H33" s="74"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="62"/>
       <c r="L33" s="19"/>
       <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="64"/>
       <c r="L34" s="19"/>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="76"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="64"/>
       <c r="L35" s="19"/>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="77" t="s">
+      <c r="F36" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="77"/>
-      <c r="H36" s="78"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="66"/>
       <c r="L36" s="19"/>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="78"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="66"/>
       <c r="L37" s="19"/>
       <c r="P37" s="19"/>
     </row>
@@ -4820,2463 +4702,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U106"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" customWidth="1"/>
-    <col min="15" max="15" width="31.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="110" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-    </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="106"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="107"/>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="109"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="90" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="116" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="85" t="s">
-        <v>72</v>
-      </c>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="86"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="87"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="117"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="89"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="141" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="141"/>
-      <c r="H9" s="142"/>
-      <c r="I9" s="143" t="s">
-        <v>99</v>
-      </c>
-      <c r="J9" s="139"/>
-      <c r="K9" s="139" t="s">
-        <v>100</v>
-      </c>
-      <c r="L9" s="140"/>
-      <c r="M9" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="N9" s="44"/>
-      <c r="O9" s="137" t="s">
-        <v>105</v>
-      </c>
-      <c r="P9" s="138"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="127" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="127"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
-      <c r="H10" s="130"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="118"/>
-      <c r="K10" s="118"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="127" t="s">
-        <v>106</v>
-      </c>
-      <c r="P10" s="128"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
-      <c r="B11" s="127" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="133" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" s="133"/>
-      <c r="H11" s="134"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="127" t="s">
-        <v>101</v>
-      </c>
-      <c r="L11" s="128"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="127" t="s">
-        <v>107</v>
-      </c>
-      <c r="P11" s="128"/>
-    </row>
-    <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
-      <c r="B12" s="133" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="133"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="139" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="139"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="127" t="s">
-        <v>102</v>
-      </c>
-      <c r="L12" s="128"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="133" t="s">
-        <v>108</v>
-      </c>
-      <c r="P12" s="134"/>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="137"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="119"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="127" t="s">
-        <v>103</v>
-      </c>
-      <c r="L13" s="128"/>
-      <c r="M13" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="N13" s="44"/>
-      <c r="O13" s="141" t="s">
-        <v>109</v>
-      </c>
-      <c r="P13" s="142"/>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="127" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="133" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="133"/>
-      <c r="H14" s="134"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="129"/>
-      <c r="P14" s="130"/>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="127" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="127"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="141" t="s">
-        <v>89</v>
-      </c>
-      <c r="G15" s="141"/>
-      <c r="H15" s="142"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="129"/>
-      <c r="P15" s="130"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="133" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="133"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="129"/>
-      <c r="G16" s="129"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="127" t="s">
-        <v>110</v>
-      </c>
-      <c r="P16" s="128"/>
-    </row>
-    <row r="17" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="137"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="129"/>
-      <c r="G17" s="129"/>
-      <c r="H17" s="130"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="133" t="s">
-        <v>121</v>
-      </c>
-      <c r="P17" s="134"/>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="127" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="127"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="129" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="129"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="N18" s="44"/>
-      <c r="O18" s="137" t="s">
-        <v>112</v>
-      </c>
-      <c r="P18" s="138"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="127" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="129"/>
-      <c r="G19" s="129"/>
-      <c r="H19" s="130"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="127" t="s">
-        <v>113</v>
-      </c>
-      <c r="P19" s="128"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="133" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="133"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="129"/>
-      <c r="H20" s="130"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="127" t="s">
-        <v>114</v>
-      </c>
-      <c r="P20" s="128"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="137"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="135" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" s="135"/>
-      <c r="H21" s="136"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="127" t="s">
-        <v>115</v>
-      </c>
-      <c r="P21" s="128"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="127" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="127"/>
-      <c r="D22" s="128"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="135"/>
-      <c r="G22" s="135"/>
-      <c r="H22" s="136"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="127" t="s">
-        <v>117</v>
-      </c>
-      <c r="P22" s="128"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44"/>
-      <c r="B23" s="127" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="127"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="135"/>
-      <c r="G23" s="135"/>
-      <c r="H23" s="136"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="133" t="s">
-        <v>118</v>
-      </c>
-      <c r="P23" s="134"/>
-    </row>
-    <row r="24" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="46"/>
-      <c r="B24" s="133" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="133"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="135" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="135"/>
-      <c r="H24" s="136"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="N24" s="44"/>
-      <c r="O24" s="137" t="s">
-        <v>119</v>
-      </c>
-      <c r="P24" s="138"/>
-    </row>
-    <row r="25" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="137"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="135"/>
-      <c r="G25" s="135"/>
-      <c r="H25" s="136"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="133" t="s">
-        <v>120</v>
-      </c>
-      <c r="P25" s="134"/>
-    </row>
-    <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="44"/>
-      <c r="B26" s="127" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="127"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="135"/>
-      <c r="G26" s="135"/>
-      <c r="H26" s="136"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="N26" s="57"/>
-      <c r="O26" s="131" t="s">
-        <v>122</v>
-      </c>
-      <c r="P26" s="132"/>
-    </row>
-    <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
-      <c r="B27" s="127" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="127"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="129" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="129"/>
-      <c r="H27" s="130"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="N27" s="57"/>
-      <c r="O27" s="131" t="s">
-        <v>123</v>
-      </c>
-      <c r="P27" s="132"/>
-    </row>
-    <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="44"/>
-      <c r="B28" s="127" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="127"/>
-      <c r="D28" s="128"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="129"/>
-      <c r="G28" s="129"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N28" s="57"/>
-      <c r="O28" s="131" t="s">
-        <v>124</v>
-      </c>
-      <c r="P28" s="132"/>
-    </row>
-    <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="129"/>
-      <c r="G29" s="129"/>
-      <c r="H29" s="130"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="N29" s="57"/>
-      <c r="O29" s="131" t="s">
-        <v>125</v>
-      </c>
-      <c r="P29" s="132"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="118" t="s">
-        <v>94</v>
-      </c>
-      <c r="G30" s="118"/>
-      <c r="H30" s="119"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="N30" s="48"/>
-      <c r="O30" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="P30" s="45"/>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="120"/>
-      <c r="G31" s="120"/>
-      <c r="H31" s="121"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="45"/>
-    </row>
-    <row r="32" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="19"/>
-      <c r="E32" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="F32" s="57" t="s">
-        <v>95</v>
-      </c>
-      <c r="G32" s="57"/>
-      <c r="H32" s="58"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="48"/>
-      <c r="P32" s="47"/>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="19"/>
-      <c r="E33" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="122" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="122"/>
-      <c r="H33" s="123"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
-      <c r="O33" s="48"/>
-      <c r="P33" s="47"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D34" s="19"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="124"/>
-      <c r="G34" s="124"/>
-      <c r="H34" s="125"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="47"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D35" s="19"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="124"/>
-      <c r="H35" s="125"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
-      <c r="P35" s="47"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D36" s="19"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="126" t="s">
-        <v>98</v>
-      </c>
-      <c r="G36" s="126"/>
-      <c r="H36" s="119"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="47"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D37" s="19"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="126"/>
-      <c r="G37" s="126"/>
-      <c r="H37" s="119"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="48"/>
-      <c r="O37" s="48"/>
-      <c r="P37" s="47"/>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="46"/>
-      <c r="P38" s="50"/>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="18"/>
-      <c r="U48" s="18"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-      <c r="T49" s="18"/>
-      <c r="U49" s="18"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="18"/>
-      <c r="U51" s="18"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
-      <c r="N52" s="18"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="18"/>
-      <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="18"/>
-      <c r="U52" s="18"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="18"/>
-      <c r="N53" s="18"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="18"/>
-      <c r="U53" s="18"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18"/>
-      <c r="O54" s="18"/>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="18"/>
-      <c r="U54" s="18"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="18"/>
-      <c r="O55" s="18"/>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="18"/>
-      <c r="U55" s="18"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="18"/>
-      <c r="T56" s="18"/>
-      <c r="U56" s="18"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="18"/>
-      <c r="R57" s="18"/>
-      <c r="S57" s="18"/>
-      <c r="T57" s="18"/>
-      <c r="U57" s="18"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
-      <c r="M58" s="18"/>
-      <c r="N58" s="18"/>
-      <c r="O58" s="18"/>
-      <c r="P58" s="18"/>
-      <c r="Q58" s="18"/>
-      <c r="R58" s="18"/>
-      <c r="S58" s="18"/>
-      <c r="T58" s="18"/>
-      <c r="U58" s="18"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="18"/>
-      <c r="L59" s="18"/>
-      <c r="M59" s="18"/>
-      <c r="N59" s="18"/>
-      <c r="O59" s="18"/>
-      <c r="P59" s="18"/>
-      <c r="Q59" s="18"/>
-      <c r="R59" s="18"/>
-      <c r="S59" s="18"/>
-      <c r="T59" s="18"/>
-      <c r="U59" s="18"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="18"/>
-      <c r="L60" s="18"/>
-      <c r="M60" s="18"/>
-      <c r="N60" s="18"/>
-      <c r="O60" s="18"/>
-      <c r="P60" s="18"/>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="18"/>
-      <c r="S60" s="18"/>
-      <c r="T60" s="18"/>
-      <c r="U60" s="18"/>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="18"/>
-      <c r="M61" s="18"/>
-      <c r="N61" s="18"/>
-      <c r="O61" s="18"/>
-      <c r="P61" s="18"/>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-      <c r="S61" s="18"/>
-      <c r="T61" s="18"/>
-      <c r="U61" s="18"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18"/>
-      <c r="N62" s="18"/>
-      <c r="O62" s="18"/>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="18"/>
-      <c r="R62" s="18"/>
-      <c r="S62" s="18"/>
-      <c r="T62" s="18"/>
-      <c r="U62" s="18"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-      <c r="L63" s="18"/>
-      <c r="M63" s="18"/>
-      <c r="N63" s="18"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="18"/>
-      <c r="Q63" s="18"/>
-      <c r="R63" s="18"/>
-      <c r="S63" s="18"/>
-      <c r="T63" s="18"/>
-      <c r="U63" s="18"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
-      <c r="L64" s="18"/>
-      <c r="M64" s="18"/>
-      <c r="N64" s="18"/>
-      <c r="O64" s="18"/>
-      <c r="P64" s="18"/>
-      <c r="Q64" s="18"/>
-      <c r="R64" s="18"/>
-      <c r="S64" s="18"/>
-      <c r="T64" s="18"/>
-      <c r="U64" s="18"/>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="18"/>
-      <c r="K65" s="18"/>
-      <c r="L65" s="18"/>
-      <c r="M65" s="18"/>
-      <c r="N65" s="18"/>
-      <c r="O65" s="18"/>
-      <c r="P65" s="18"/>
-      <c r="Q65" s="18"/>
-      <c r="R65" s="18"/>
-      <c r="S65" s="18"/>
-      <c r="T65" s="18"/>
-      <c r="U65" s="18"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
-      <c r="J66" s="18"/>
-      <c r="K66" s="18"/>
-      <c r="L66" s="18"/>
-      <c r="M66" s="18"/>
-      <c r="N66" s="18"/>
-      <c r="O66" s="18"/>
-      <c r="P66" s="18"/>
-      <c r="Q66" s="18"/>
-      <c r="R66" s="18"/>
-      <c r="S66" s="18"/>
-      <c r="T66" s="18"/>
-      <c r="U66" s="18"/>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="18"/>
-      <c r="M67" s="18"/>
-      <c r="N67" s="18"/>
-      <c r="O67" s="18"/>
-      <c r="P67" s="18"/>
-      <c r="Q67" s="18"/>
-      <c r="R67" s="18"/>
-      <c r="S67" s="18"/>
-      <c r="T67" s="18"/>
-      <c r="U67" s="18"/>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-      <c r="J68" s="18"/>
-      <c r="K68" s="18"/>
-      <c r="L68" s="18"/>
-      <c r="M68" s="18"/>
-      <c r="N68" s="18"/>
-      <c r="O68" s="18"/>
-      <c r="P68" s="18"/>
-      <c r="Q68" s="18"/>
-      <c r="R68" s="18"/>
-      <c r="S68" s="18"/>
-      <c r="T68" s="18"/>
-      <c r="U68" s="18"/>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-      <c r="L69" s="18"/>
-      <c r="M69" s="18"/>
-      <c r="N69" s="18"/>
-      <c r="O69" s="18"/>
-      <c r="P69" s="18"/>
-      <c r="Q69" s="18"/>
-      <c r="R69" s="18"/>
-      <c r="S69" s="18"/>
-      <c r="T69" s="18"/>
-      <c r="U69" s="18"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="18"/>
-      <c r="K70" s="18"/>
-      <c r="L70" s="18"/>
-      <c r="M70" s="18"/>
-      <c r="N70" s="18"/>
-      <c r="O70" s="18"/>
-      <c r="P70" s="18"/>
-      <c r="Q70" s="18"/>
-      <c r="R70" s="18"/>
-      <c r="S70" s="18"/>
-      <c r="T70" s="18"/>
-      <c r="U70" s="18"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="18"/>
-      <c r="L71" s="18"/>
-      <c r="M71" s="18"/>
-      <c r="N71" s="18"/>
-      <c r="O71" s="18"/>
-      <c r="P71" s="18"/>
-      <c r="Q71" s="18"/>
-      <c r="R71" s="18"/>
-      <c r="S71" s="18"/>
-      <c r="T71" s="18"/>
-      <c r="U71" s="18"/>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
-      <c r="L72" s="18"/>
-      <c r="M72" s="18"/>
-      <c r="N72" s="18"/>
-      <c r="O72" s="18"/>
-      <c r="P72" s="18"/>
-      <c r="Q72" s="18"/>
-      <c r="R72" s="18"/>
-      <c r="S72" s="18"/>
-      <c r="T72" s="18"/>
-      <c r="U72" s="18"/>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="18"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="18"/>
-      <c r="L73" s="18"/>
-      <c r="M73" s="18"/>
-      <c r="N73" s="18"/>
-      <c r="O73" s="18"/>
-      <c r="P73" s="18"/>
-      <c r="Q73" s="18"/>
-      <c r="R73" s="18"/>
-      <c r="S73" s="18"/>
-      <c r="T73" s="18"/>
-      <c r="U73" s="18"/>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="18"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="L74" s="18"/>
-      <c r="M74" s="18"/>
-      <c r="N74" s="18"/>
-      <c r="O74" s="18"/>
-      <c r="P74" s="18"/>
-      <c r="Q74" s="18"/>
-      <c r="R74" s="18"/>
-      <c r="S74" s="18"/>
-      <c r="T74" s="18"/>
-      <c r="U74" s="18"/>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="18"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="18"/>
-      <c r="L75" s="18"/>
-      <c r="M75" s="18"/>
-      <c r="N75" s="18"/>
-      <c r="O75" s="18"/>
-      <c r="P75" s="18"/>
-      <c r="Q75" s="18"/>
-      <c r="R75" s="18"/>
-      <c r="S75" s="18"/>
-      <c r="T75" s="18"/>
-      <c r="U75" s="18"/>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-      <c r="L76" s="18"/>
-      <c r="M76" s="18"/>
-      <c r="N76" s="18"/>
-      <c r="O76" s="18"/>
-      <c r="P76" s="18"/>
-      <c r="Q76" s="18"/>
-      <c r="R76" s="18"/>
-      <c r="S76" s="18"/>
-      <c r="T76" s="18"/>
-      <c r="U76" s="18"/>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A77" s="18"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
-      <c r="K77" s="18"/>
-      <c r="L77" s="18"/>
-      <c r="M77" s="18"/>
-      <c r="N77" s="18"/>
-      <c r="O77" s="18"/>
-      <c r="P77" s="18"/>
-      <c r="Q77" s="18"/>
-      <c r="R77" s="18"/>
-      <c r="S77" s="18"/>
-      <c r="T77" s="18"/>
-      <c r="U77" s="18"/>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="18"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
-      <c r="K78" s="18"/>
-      <c r="L78" s="18"/>
-      <c r="M78" s="18"/>
-      <c r="N78" s="18"/>
-      <c r="O78" s="18"/>
-      <c r="P78" s="18"/>
-      <c r="Q78" s="18"/>
-      <c r="R78" s="18"/>
-      <c r="S78" s="18"/>
-      <c r="T78" s="18"/>
-      <c r="U78" s="18"/>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
-      <c r="J79" s="18"/>
-      <c r="K79" s="18"/>
-      <c r="L79" s="18"/>
-      <c r="M79" s="18"/>
-      <c r="N79" s="18"/>
-      <c r="O79" s="18"/>
-      <c r="P79" s="18"/>
-      <c r="Q79" s="18"/>
-      <c r="R79" s="18"/>
-      <c r="S79" s="18"/>
-      <c r="T79" s="18"/>
-      <c r="U79" s="18"/>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="18"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="18"/>
-      <c r="L80" s="18"/>
-      <c r="M80" s="18"/>
-      <c r="N80" s="18"/>
-      <c r="O80" s="18"/>
-      <c r="P80" s="18"/>
-      <c r="Q80" s="18"/>
-      <c r="R80" s="18"/>
-      <c r="S80" s="18"/>
-      <c r="T80" s="18"/>
-      <c r="U80" s="18"/>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="18"/>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="18"/>
-      <c r="K81" s="18"/>
-      <c r="L81" s="18"/>
-      <c r="M81" s="18"/>
-      <c r="N81" s="18"/>
-      <c r="O81" s="18"/>
-      <c r="P81" s="18"/>
-      <c r="Q81" s="18"/>
-      <c r="R81" s="18"/>
-      <c r="S81" s="18"/>
-      <c r="T81" s="18"/>
-      <c r="U81" s="18"/>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
-      <c r="J82" s="18"/>
-      <c r="K82" s="18"/>
-      <c r="L82" s="18"/>
-      <c r="M82" s="18"/>
-      <c r="N82" s="18"/>
-      <c r="O82" s="18"/>
-      <c r="P82" s="18"/>
-      <c r="Q82" s="18"/>
-      <c r="R82" s="18"/>
-      <c r="S82" s="18"/>
-      <c r="T82" s="18"/>
-      <c r="U82" s="18"/>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="18"/>
-      <c r="H83" s="18"/>
-      <c r="I83" s="18"/>
-      <c r="J83" s="18"/>
-      <c r="K83" s="18"/>
-      <c r="L83" s="18"/>
-      <c r="M83" s="18"/>
-      <c r="N83" s="18"/>
-      <c r="O83" s="18"/>
-      <c r="P83" s="18"/>
-      <c r="Q83" s="18"/>
-      <c r="R83" s="18"/>
-      <c r="S83" s="18"/>
-      <c r="T83" s="18"/>
-      <c r="U83" s="18"/>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
-      <c r="J84" s="18"/>
-      <c r="K84" s="18"/>
-      <c r="L84" s="18"/>
-      <c r="M84" s="18"/>
-      <c r="N84" s="18"/>
-      <c r="O84" s="18"/>
-      <c r="P84" s="18"/>
-      <c r="Q84" s="18"/>
-      <c r="R84" s="18"/>
-      <c r="S84" s="18"/>
-      <c r="T84" s="18"/>
-      <c r="U84" s="18"/>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="18"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18"/>
-      <c r="I85" s="18"/>
-      <c r="J85" s="18"/>
-      <c r="K85" s="18"/>
-      <c r="L85" s="18"/>
-      <c r="M85" s="18"/>
-      <c r="N85" s="18"/>
-      <c r="O85" s="18"/>
-      <c r="P85" s="18"/>
-      <c r="Q85" s="18"/>
-      <c r="R85" s="18"/>
-      <c r="S85" s="18"/>
-      <c r="T85" s="18"/>
-      <c r="U85" s="18"/>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="18"/>
-      <c r="J86" s="18"/>
-      <c r="K86" s="18"/>
-      <c r="L86" s="18"/>
-      <c r="M86" s="18"/>
-      <c r="N86" s="18"/>
-      <c r="O86" s="18"/>
-      <c r="P86" s="18"/>
-      <c r="Q86" s="18"/>
-      <c r="R86" s="18"/>
-      <c r="S86" s="18"/>
-      <c r="T86" s="18"/>
-      <c r="U86" s="18"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A87" s="18"/>
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
-      <c r="I87" s="18"/>
-      <c r="J87" s="18"/>
-      <c r="K87" s="18"/>
-      <c r="L87" s="18"/>
-      <c r="M87" s="18"/>
-      <c r="N87" s="18"/>
-      <c r="O87" s="18"/>
-      <c r="P87" s="18"/>
-      <c r="Q87" s="18"/>
-      <c r="R87" s="18"/>
-      <c r="S87" s="18"/>
-      <c r="T87" s="18"/>
-      <c r="U87" s="18"/>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
-      <c r="B88" s="18"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
-      <c r="J88" s="18"/>
-      <c r="K88" s="18"/>
-      <c r="L88" s="18"/>
-      <c r="M88" s="18"/>
-      <c r="N88" s="18"/>
-      <c r="O88" s="18"/>
-      <c r="P88" s="18"/>
-      <c r="Q88" s="18"/>
-      <c r="R88" s="18"/>
-      <c r="S88" s="18"/>
-      <c r="T88" s="18"/>
-      <c r="U88" s="18"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A89" s="18"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="18"/>
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="18"/>
-      <c r="M89" s="18"/>
-      <c r="N89" s="18"/>
-      <c r="O89" s="18"/>
-      <c r="P89" s="18"/>
-      <c r="Q89" s="18"/>
-      <c r="R89" s="18"/>
-      <c r="S89" s="18"/>
-      <c r="T89" s="18"/>
-      <c r="U89" s="18"/>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A90" s="18"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
-      <c r="J90" s="18"/>
-      <c r="K90" s="18"/>
-      <c r="L90" s="18"/>
-      <c r="M90" s="18"/>
-      <c r="N90" s="18"/>
-      <c r="O90" s="18"/>
-      <c r="P90" s="18"/>
-      <c r="Q90" s="18"/>
-      <c r="R90" s="18"/>
-      <c r="S90" s="18"/>
-      <c r="T90" s="18"/>
-      <c r="U90" s="18"/>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A91" s="18"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="18"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
-      <c r="J91" s="18"/>
-      <c r="K91" s="18"/>
-      <c r="L91" s="18"/>
-      <c r="M91" s="18"/>
-      <c r="N91" s="18"/>
-      <c r="O91" s="18"/>
-      <c r="P91" s="18"/>
-      <c r="Q91" s="18"/>
-      <c r="R91" s="18"/>
-      <c r="S91" s="18"/>
-      <c r="T91" s="18"/>
-      <c r="U91" s="18"/>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="18"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
-      <c r="J92" s="18"/>
-      <c r="K92" s="18"/>
-      <c r="L92" s="18"/>
-      <c r="M92" s="18"/>
-      <c r="N92" s="18"/>
-      <c r="O92" s="18"/>
-      <c r="P92" s="18"/>
-      <c r="Q92" s="18"/>
-      <c r="R92" s="18"/>
-      <c r="S92" s="18"/>
-      <c r="T92" s="18"/>
-      <c r="U92" s="18"/>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="18"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="18"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
-      <c r="J93" s="18"/>
-      <c r="K93" s="18"/>
-      <c r="L93" s="18"/>
-      <c r="M93" s="18"/>
-      <c r="N93" s="18"/>
-      <c r="O93" s="18"/>
-      <c r="P93" s="18"/>
-      <c r="Q93" s="18"/>
-      <c r="R93" s="18"/>
-      <c r="S93" s="18"/>
-      <c r="T93" s="18"/>
-      <c r="U93" s="18"/>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="18"/>
-      <c r="C94" s="18"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
-      <c r="J94" s="18"/>
-      <c r="K94" s="18"/>
-      <c r="L94" s="18"/>
-      <c r="M94" s="18"/>
-      <c r="N94" s="18"/>
-      <c r="O94" s="18"/>
-      <c r="P94" s="18"/>
-      <c r="Q94" s="18"/>
-      <c r="R94" s="18"/>
-      <c r="S94" s="18"/>
-      <c r="T94" s="18"/>
-      <c r="U94" s="18"/>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
-      <c r="J95" s="18"/>
-      <c r="K95" s="18"/>
-      <c r="L95" s="18"/>
-      <c r="M95" s="18"/>
-      <c r="N95" s="18"/>
-      <c r="O95" s="18"/>
-      <c r="P95" s="18"/>
-      <c r="Q95" s="18"/>
-      <c r="R95" s="18"/>
-      <c r="S95" s="18"/>
-      <c r="T95" s="18"/>
-      <c r="U95" s="18"/>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A96" s="18"/>
-      <c r="B96" s="18"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="18"/>
-      <c r="H96" s="18"/>
-      <c r="I96" s="18"/>
-      <c r="J96" s="18"/>
-      <c r="K96" s="18"/>
-      <c r="L96" s="18"/>
-      <c r="M96" s="18"/>
-      <c r="N96" s="18"/>
-      <c r="O96" s="18"/>
-      <c r="P96" s="18"/>
-      <c r="Q96" s="18"/>
-      <c r="R96" s="18"/>
-      <c r="S96" s="18"/>
-      <c r="T96" s="18"/>
-      <c r="U96" s="18"/>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="18"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
-      <c r="J97" s="18"/>
-      <c r="K97" s="18"/>
-      <c r="L97" s="18"/>
-      <c r="M97" s="18"/>
-      <c r="N97" s="18"/>
-      <c r="O97" s="18"/>
-      <c r="P97" s="18"/>
-      <c r="Q97" s="18"/>
-      <c r="R97" s="18"/>
-      <c r="S97" s="18"/>
-      <c r="T97" s="18"/>
-      <c r="U97" s="18"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A98" s="18"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
-      <c r="I98" s="18"/>
-      <c r="J98" s="18"/>
-      <c r="K98" s="18"/>
-      <c r="L98" s="18"/>
-      <c r="M98" s="18"/>
-      <c r="N98" s="18"/>
-      <c r="O98" s="18"/>
-      <c r="P98" s="18"/>
-      <c r="Q98" s="18"/>
-      <c r="R98" s="18"/>
-      <c r="S98" s="18"/>
-      <c r="T98" s="18"/>
-      <c r="U98" s="18"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A99" s="18"/>
-      <c r="B99" s="18"/>
-      <c r="C99" s="18"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="18"/>
-      <c r="H99" s="18"/>
-      <c r="I99" s="18"/>
-      <c r="J99" s="18"/>
-      <c r="K99" s="18"/>
-      <c r="L99" s="18"/>
-      <c r="M99" s="18"/>
-      <c r="N99" s="18"/>
-      <c r="O99" s="18"/>
-      <c r="P99" s="18"/>
-      <c r="Q99" s="18"/>
-      <c r="R99" s="18"/>
-      <c r="S99" s="18"/>
-      <c r="T99" s="18"/>
-      <c r="U99" s="18"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A100" s="18"/>
-      <c r="B100" s="18"/>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="18"/>
-      <c r="I100" s="18"/>
-      <c r="J100" s="18"/>
-      <c r="K100" s="18"/>
-      <c r="L100" s="18"/>
-      <c r="M100" s="18"/>
-      <c r="N100" s="18"/>
-      <c r="O100" s="18"/>
-      <c r="P100" s="18"/>
-      <c r="Q100" s="18"/>
-      <c r="R100" s="18"/>
-      <c r="S100" s="18"/>
-      <c r="T100" s="18"/>
-      <c r="U100" s="18"/>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A101" s="18"/>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="18"/>
-      <c r="H101" s="18"/>
-      <c r="I101" s="18"/>
-      <c r="J101" s="18"/>
-      <c r="K101" s="18"/>
-      <c r="L101" s="18"/>
-      <c r="M101" s="18"/>
-      <c r="N101" s="18"/>
-      <c r="O101" s="18"/>
-      <c r="P101" s="18"/>
-      <c r="Q101" s="18"/>
-      <c r="R101" s="18"/>
-      <c r="S101" s="18"/>
-      <c r="T101" s="18"/>
-      <c r="U101" s="18"/>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A102" s="18"/>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
-      <c r="J102" s="18"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="18"/>
-      <c r="M102" s="18"/>
-      <c r="N102" s="18"/>
-      <c r="O102" s="18"/>
-      <c r="P102" s="18"/>
-      <c r="Q102" s="18"/>
-      <c r="R102" s="18"/>
-      <c r="S102" s="18"/>
-      <c r="T102" s="18"/>
-      <c r="U102" s="18"/>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="18"/>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
-      <c r="J103" s="18"/>
-      <c r="K103" s="18"/>
-      <c r="L103" s="18"/>
-      <c r="M103" s="18"/>
-      <c r="N103" s="18"/>
-      <c r="O103" s="18"/>
-      <c r="P103" s="18"/>
-      <c r="Q103" s="18"/>
-      <c r="R103" s="18"/>
-      <c r="S103" s="18"/>
-      <c r="T103" s="18"/>
-      <c r="U103" s="18"/>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A104" s="18"/>
-      <c r="B104" s="18"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
-      <c r="H104" s="18"/>
-      <c r="I104" s="18"/>
-      <c r="J104" s="18"/>
-      <c r="K104" s="18"/>
-      <c r="L104" s="18"/>
-      <c r="M104" s="18"/>
-      <c r="N104" s="18"/>
-      <c r="O104" s="18"/>
-      <c r="P104" s="18"/>
-      <c r="Q104" s="18"/>
-      <c r="R104" s="18"/>
-      <c r="S104" s="18"/>
-      <c r="T104" s="18"/>
-      <c r="U104" s="18"/>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A105" s="18"/>
-      <c r="B105" s="18"/>
-      <c r="C105" s="18"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-      <c r="H105" s="18"/>
-      <c r="I105" s="18"/>
-      <c r="J105" s="18"/>
-      <c r="K105" s="18"/>
-      <c r="L105" s="18"/>
-      <c r="M105" s="18"/>
-      <c r="N105" s="18"/>
-      <c r="O105" s="18"/>
-      <c r="P105" s="18"/>
-      <c r="Q105" s="18"/>
-      <c r="R105" s="18"/>
-      <c r="S105" s="18"/>
-      <c r="T105" s="18"/>
-      <c r="U105" s="18"/>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A106" s="18"/>
-      <c r="B106" s="18"/>
-      <c r="C106" s="18"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="18"/>
-      <c r="I106" s="18"/>
-      <c r="J106" s="18"/>
-      <c r="K106" s="18"/>
-      <c r="L106" s="18"/>
-      <c r="M106" s="18"/>
-      <c r="N106" s="18"/>
-      <c r="O106" s="18"/>
-      <c r="P106" s="18"/>
-      <c r="Q106" s="18"/>
-      <c r="R106" s="18"/>
-      <c r="S106" s="18"/>
-      <c r="T106" s="18"/>
-      <c r="U106" s="18"/>
-    </row>
-  </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="A2:P3"/>
-    <mergeCell ref="A4:H6"/>
-    <mergeCell ref="I4:P6"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F12:H13"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="O13:P15"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="F15:H17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H29"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Avance funcionalidad de mostrar los articulos del carrito en layout
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
     <sheet name="Modulos Y Mantenimientos" sheetId="2" r:id="rId2"/>
+    <sheet name="Modulos Y Mantenimientos ESTADO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="133">
   <si>
     <t>Nombre</t>
   </si>
@@ -415,6 +416,12 @@
   </si>
   <si>
     <t>Muestra info del usuario, cambio clave</t>
+  </si>
+  <si>
+    <t>CASI TERMINADO</t>
+  </si>
+  <si>
+    <t>Terminado</t>
   </si>
 </sst>
 </file>
@@ -461,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +490,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -794,181 +807,237 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2303,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
@@ -2320,259 +2389,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="88"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="77"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="91"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="80"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="98" t="s">
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="94"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="83"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="94"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="83"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="95"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="96"/>
-      <c r="L6" s="96"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="97"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="86"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="78" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="104" t="s">
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="73" t="s">
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="74"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="61"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="77"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="64"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="100"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="80" t="s">
+      <c r="F9" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="80"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="100" t="s">
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84" t="s">
+      <c r="J9" s="71"/>
+      <c r="K9" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="85"/>
+      <c r="L9" s="72"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="57" t="s">
+      <c r="O9" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="58"/>
+      <c r="P9" s="100"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="109"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="66"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="74"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="59" t="s">
+      <c r="O10" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="60"/>
+      <c r="P10" s="109"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="109"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="96"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="59" t="s">
+      <c r="K11" s="108" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="60"/>
+      <c r="L11" s="109"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="59" t="s">
+      <c r="O11" s="108" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="60"/>
+      <c r="P11" s="109"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="60"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="84" t="s">
+      <c r="F12" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="84"/>
-      <c r="H12" s="85"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="59" t="s">
+      <c r="K12" s="108" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="60"/>
+      <c r="L12" s="109"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="55" t="s">
+      <c r="O12" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="56"/>
+      <c r="P12" s="96"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -2581,23 +2650,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="66"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="74"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="59" t="s">
+      <c r="K13" s="108" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="60"/>
+      <c r="L13" s="109"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="80" t="s">
+      <c r="O13" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="81"/>
+      <c r="P13" s="68"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -2609,19 +2678,19 @@
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="55"/>
-      <c r="H14" s="56"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="96"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="32"/>
       <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="83"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="70"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2633,19 +2702,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="102" t="s">
+      <c r="F15" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="92"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="82"/>
-      <c r="P15" s="83"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="70"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -2655,19 +2724,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="31"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="94"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="49" t="s">
+      <c r="O16" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="50"/>
+      <c r="P16" s="111"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -2677,19 +2746,19 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="94"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="55" t="s">
+      <c r="O17" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="56"/>
+      <c r="P17" s="96"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2701,11 +2770,11 @@
       <c r="C18" s="36"/>
       <c r="D18" s="37"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="67" t="s">
+      <c r="F18" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="67"/>
-      <c r="H18" s="68"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="94"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -2714,10 +2783,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="53" t="s">
+      <c r="O18" s="112" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="54"/>
+      <c r="P18" s="113"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -2727,19 +2796,19 @@
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="94"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="49" t="s">
+      <c r="O19" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="50"/>
+      <c r="P19" s="111"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -2749,19 +2818,19 @@
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="68"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="94"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="49" t="s">
+      <c r="O20" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="50"/>
+      <c r="P20" s="111"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -2771,21 +2840,21 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="69" t="s">
+      <c r="F21" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="69"/>
-      <c r="H21" s="66"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="74"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="49" t="s">
+      <c r="O21" s="110" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="50"/>
+      <c r="P21" s="111"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2797,19 +2866,19 @@
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="66"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="49" t="s">
+      <c r="O22" s="110" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="50"/>
+      <c r="P22" s="111"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -2819,19 +2888,19 @@
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="66"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="74"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="51" t="s">
+      <c r="O23" s="116" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="52"/>
+      <c r="P23" s="117"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -2841,11 +2910,11 @@
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="69" t="s">
+      <c r="F24" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="69"/>
-      <c r="H24" s="66"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="74"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -2854,10 +2923,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="53" t="s">
+      <c r="O24" s="112" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="54"/>
+      <c r="P24" s="113"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -2867,19 +2936,19 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="66"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="74"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="51" t="s">
+      <c r="O25" s="116" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="52"/>
+      <c r="P25" s="117"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -2891,9 +2960,9 @@
       <c r="C26" s="36"/>
       <c r="D26" s="37"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="66"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="74"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -2902,10 +2971,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="25"/>
-      <c r="O26" s="47" t="s">
+      <c r="O26" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="48"/>
+      <c r="P26" s="115"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -2915,11 +2984,11 @@
       <c r="C27" s="38"/>
       <c r="D27" s="39"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="67" t="s">
+      <c r="F27" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="67"/>
-      <c r="H27" s="68"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="94"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -2928,10 +2997,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="47" t="s">
+      <c r="O27" s="114" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="48"/>
+      <c r="P27" s="115"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -2941,9 +3010,9 @@
       <c r="C28" s="38"/>
       <c r="D28" s="39"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="68"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="94"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -2952,10 +3021,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="47" t="s">
+      <c r="O28" s="114" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="48"/>
+      <c r="P28" s="115"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -2965,9 +3034,9 @@
       <c r="C29" s="38"/>
       <c r="D29" s="39"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="68"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="94"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -2976,18 +3045,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="47" t="s">
+      <c r="O29" s="114" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="48"/>
+      <c r="P29" s="115"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="69" t="s">
+      <c r="F30" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="69"/>
-      <c r="H30" s="66"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="74"/>
       <c r="L30" s="19"/>
       <c r="M30" s="23" t="s">
         <v>125</v>
@@ -3000,9 +3069,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="71"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="107"/>
       <c r="L31" s="19"/>
       <c r="O31" s="30"/>
       <c r="P31" s="31"/>
@@ -3025,45 +3094,45 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="61" t="s">
+      <c r="F33" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="61"/>
-      <c r="H33" s="62"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="102"/>
       <c r="L33" s="19"/>
       <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="64"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="104"/>
       <c r="L34" s="19"/>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="103"/>
+      <c r="H35" s="104"/>
       <c r="L35" s="19"/>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="65" t="s">
+      <c r="F36" s="105" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="65"/>
-      <c r="H36" s="66"/>
+      <c r="G36" s="105"/>
+      <c r="H36" s="74"/>
       <c r="L36" s="19"/>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="66"/>
+      <c r="F37" s="105"/>
+      <c r="G37" s="105"/>
+      <c r="H37" s="74"/>
       <c r="L37" s="19"/>
       <c r="P37" s="19"/>
     </row>
@@ -4651,6 +4720,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="F30:H31"/>
     <mergeCell ref="A7:D8"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="F9:H10"/>
@@ -4667,37 +4767,2438 @@
     <mergeCell ref="I7:L8"/>
     <mergeCell ref="M7:P8"/>
     <mergeCell ref="B9:D9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="31.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="78"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+    </row>
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="81"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="83"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="86"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="61"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="62"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="64"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="99" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="99"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="72"/>
+      <c r="M9" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="N9" s="18"/>
+      <c r="O9" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="P9" s="100"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="108" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="108"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="108" t="s">
+        <v>106</v>
+      </c>
+      <c r="P10" s="109"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="108" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="108"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="95"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="108" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="109"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="108" t="s">
+        <v>107</v>
+      </c>
+      <c r="P11" s="109"/>
+    </row>
+    <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="108" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" s="109"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="P12" s="96"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="108" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="109"/>
+      <c r="M13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="18"/>
+      <c r="O13" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P13" s="68"/>
+    </row>
+    <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="95"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="70"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="57"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="91"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="70"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="57"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="110" t="s">
+        <v>110</v>
+      </c>
+      <c r="P16" s="111"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="95" t="s">
+        <v>121</v>
+      </c>
+      <c r="P17" s="96"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="93"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="N18" s="18"/>
+      <c r="O18" s="112" t="s">
+        <v>112</v>
+      </c>
+      <c r="P18" s="113"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="110" t="s">
+        <v>113</v>
+      </c>
+      <c r="P19" s="111"/>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="110" t="s">
+        <v>114</v>
+      </c>
+      <c r="P20" s="111"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+      <c r="B21" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="73"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="110" t="s">
+        <v>115</v>
+      </c>
+      <c r="P21" s="111"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="P22" s="111"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="P23" s="117"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="73"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="N24" s="18"/>
+      <c r="O24" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="P24" s="113"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="116" t="s">
+        <v>120</v>
+      </c>
+      <c r="P25" s="117"/>
+    </row>
+    <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="N26" s="25"/>
+      <c r="O26" s="114" t="s">
+        <v>130</v>
+      </c>
+      <c r="P26" s="115"/>
+    </row>
+    <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="93" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="93"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="N27" s="25"/>
+      <c r="O27" s="114" t="s">
+        <v>122</v>
+      </c>
+      <c r="P27" s="115"/>
+    </row>
+    <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="N28" s="25"/>
+      <c r="O28" s="114" t="s">
+        <v>123</v>
+      </c>
+      <c r="P28" s="115"/>
+    </row>
+    <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="N29" s="25"/>
+      <c r="O29" s="114" t="s">
+        <v>124</v>
+      </c>
+      <c r="P29" s="115"/>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="19"/>
+      <c r="F30" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="73"/>
+      <c r="H30" s="74"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="118" t="s">
+        <v>125</v>
+      </c>
+      <c r="N30" s="119"/>
+      <c r="O30" s="120" t="s">
+        <v>126</v>
+      </c>
+      <c r="P30" s="121"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="19"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="107"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="120"/>
+      <c r="P31" s="121"/>
+    </row>
+    <row r="32" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="19"/>
+      <c r="E32" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="25"/>
+      <c r="H32" s="26"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="119"/>
+      <c r="N32" s="119"/>
+      <c r="O32" s="119"/>
+      <c r="P32" s="122"/>
+    </row>
+    <row r="33" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="19"/>
+      <c r="E33" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="G33" s="101"/>
+      <c r="H33" s="102"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="119"/>
+      <c r="N33" s="119"/>
+      <c r="O33" s="119"/>
+      <c r="P33" s="122"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D34" s="19"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="104"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="119"/>
+      <c r="N34" s="119"/>
+      <c r="O34" s="119"/>
+      <c r="P34" s="122"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D35" s="19"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="103"/>
+      <c r="H35" s="104"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="119"/>
+      <c r="N35" s="119"/>
+      <c r="O35" s="119"/>
+      <c r="P35" s="122"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D36" s="19"/>
+      <c r="F36" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="105"/>
+      <c r="H36" s="74"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="119"/>
+      <c r="N36" s="119"/>
+      <c r="O36" s="119"/>
+      <c r="P36" s="122"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D37" s="19"/>
+      <c r="F37" s="105"/>
+      <c r="G37" s="105"/>
+      <c r="H37" s="74"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="119"/>
+      <c r="N37" s="119"/>
+      <c r="O37" s="119"/>
+      <c r="P37" s="122"/>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="123"/>
+      <c r="N38" s="123"/>
+      <c r="O38" s="123"/>
+      <c r="P38" s="124"/>
+    </row>
+    <row r="39" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="125" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" s="126"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="127" t="s">
+        <v>132</v>
+      </c>
+      <c r="I41" s="127"/>
+      <c r="J41" s="127"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="126"/>
+      <c r="F42" s="126"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="127"/>
+      <c r="I42" s="127"/>
+      <c r="J42" s="127"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="18"/>
+      <c r="U43" s="18"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="18"/>
+      <c r="U44" s="18"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18"/>
+      <c r="U45" s="18"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="18"/>
+      <c r="U46" s="18"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="18"/>
+      <c r="U47" s="18"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="18"/>
+      <c r="U48" s="18"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="18"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="18"/>
+      <c r="U50" s="18"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
+      <c r="S51" s="18"/>
+      <c r="T51" s="18"/>
+      <c r="U51" s="18"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="18"/>
+      <c r="U52" s="18"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="18"/>
+      <c r="U53" s="18"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="18"/>
+      <c r="Q54" s="18"/>
+      <c r="R54" s="18"/>
+      <c r="S54" s="18"/>
+      <c r="T54" s="18"/>
+      <c r="U54" s="18"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="18"/>
+      <c r="U55" s="18"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="18"/>
+      <c r="U56" s="18"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="18"/>
+      <c r="U57" s="18"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="18"/>
+      <c r="Q58" s="18"/>
+      <c r="R58" s="18"/>
+      <c r="S58" s="18"/>
+      <c r="T58" s="18"/>
+      <c r="U58" s="18"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="18"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="18"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" s="18"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="18"/>
+      <c r="U59" s="18"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="18"/>
+      <c r="Q60" s="18"/>
+      <c r="R60" s="18"/>
+      <c r="S60" s="18"/>
+      <c r="T60" s="18"/>
+      <c r="U60" s="18"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+      <c r="T61" s="18"/>
+      <c r="U61" s="18"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" s="18"/>
+      <c r="S62" s="18"/>
+      <c r="T62" s="18"/>
+      <c r="U62" s="18"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="18"/>
+      <c r="R63" s="18"/>
+      <c r="S63" s="18"/>
+      <c r="T63" s="18"/>
+      <c r="U63" s="18"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
+      <c r="P64" s="18"/>
+      <c r="Q64" s="18"/>
+      <c r="R64" s="18"/>
+      <c r="S64" s="18"/>
+      <c r="T64" s="18"/>
+      <c r="U64" s="18"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18"/>
+      <c r="S65" s="18"/>
+      <c r="T65" s="18"/>
+      <c r="U65" s="18"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="18"/>
+      <c r="Q66" s="18"/>
+      <c r="R66" s="18"/>
+      <c r="S66" s="18"/>
+      <c r="T66" s="18"/>
+      <c r="U66" s="18"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="18"/>
+      <c r="R67" s="18"/>
+      <c r="S67" s="18"/>
+      <c r="T67" s="18"/>
+      <c r="U67" s="18"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+      <c r="M68" s="18"/>
+      <c r="N68" s="18"/>
+      <c r="O68" s="18"/>
+      <c r="P68" s="18"/>
+      <c r="Q68" s="18"/>
+      <c r="R68" s="18"/>
+      <c r="S68" s="18"/>
+      <c r="T68" s="18"/>
+      <c r="U68" s="18"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="18"/>
+      <c r="P69" s="18"/>
+      <c r="Q69" s="18"/>
+      <c r="R69" s="18"/>
+      <c r="S69" s="18"/>
+      <c r="T69" s="18"/>
+      <c r="U69" s="18"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="18"/>
+      <c r="M70" s="18"/>
+      <c r="N70" s="18"/>
+      <c r="O70" s="18"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="18"/>
+      <c r="R70" s="18"/>
+      <c r="S70" s="18"/>
+      <c r="T70" s="18"/>
+      <c r="U70" s="18"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="18"/>
+      <c r="M71" s="18"/>
+      <c r="N71" s="18"/>
+      <c r="O71" s="18"/>
+      <c r="P71" s="18"/>
+      <c r="Q71" s="18"/>
+      <c r="R71" s="18"/>
+      <c r="S71" s="18"/>
+      <c r="T71" s="18"/>
+      <c r="U71" s="18"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="18"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="18"/>
+      <c r="M72" s="18"/>
+      <c r="N72" s="18"/>
+      <c r="O72" s="18"/>
+      <c r="P72" s="18"/>
+      <c r="Q72" s="18"/>
+      <c r="R72" s="18"/>
+      <c r="S72" s="18"/>
+      <c r="T72" s="18"/>
+      <c r="U72" s="18"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="18"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="18"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="18"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
+      <c r="S73" s="18"/>
+      <c r="T73" s="18"/>
+      <c r="U73" s="18"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="18"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="18"/>
+      <c r="N74" s="18"/>
+      <c r="O74" s="18"/>
+      <c r="P74" s="18"/>
+      <c r="Q74" s="18"/>
+      <c r="R74" s="18"/>
+      <c r="S74" s="18"/>
+      <c r="T74" s="18"/>
+      <c r="U74" s="18"/>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="18"/>
+      <c r="M75" s="18"/>
+      <c r="N75" s="18"/>
+      <c r="O75" s="18"/>
+      <c r="P75" s="18"/>
+      <c r="Q75" s="18"/>
+      <c r="R75" s="18"/>
+      <c r="S75" s="18"/>
+      <c r="T75" s="18"/>
+      <c r="U75" s="18"/>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18"/>
+      <c r="M76" s="18"/>
+      <c r="N76" s="18"/>
+      <c r="O76" s="18"/>
+      <c r="P76" s="18"/>
+      <c r="Q76" s="18"/>
+      <c r="R76" s="18"/>
+      <c r="S76" s="18"/>
+      <c r="T76" s="18"/>
+      <c r="U76" s="18"/>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A77" s="18"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="18"/>
+      <c r="M77" s="18"/>
+      <c r="N77" s="18"/>
+      <c r="O77" s="18"/>
+      <c r="P77" s="18"/>
+      <c r="Q77" s="18"/>
+      <c r="R77" s="18"/>
+      <c r="S77" s="18"/>
+      <c r="T77" s="18"/>
+      <c r="U77" s="18"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="18"/>
+      <c r="R78" s="18"/>
+      <c r="S78" s="18"/>
+      <c r="T78" s="18"/>
+      <c r="U78" s="18"/>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="18"/>
+      <c r="M79" s="18"/>
+      <c r="N79" s="18"/>
+      <c r="O79" s="18"/>
+      <c r="P79" s="18"/>
+      <c r="Q79" s="18"/>
+      <c r="R79" s="18"/>
+      <c r="S79" s="18"/>
+      <c r="T79" s="18"/>
+      <c r="U79" s="18"/>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="18"/>
+      <c r="M80" s="18"/>
+      <c r="N80" s="18"/>
+      <c r="O80" s="18"/>
+      <c r="P80" s="18"/>
+      <c r="Q80" s="18"/>
+      <c r="R80" s="18"/>
+      <c r="S80" s="18"/>
+      <c r="T80" s="18"/>
+      <c r="U80" s="18"/>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A81" s="18"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="18"/>
+      <c r="R81" s="18"/>
+      <c r="S81" s="18"/>
+      <c r="T81" s="18"/>
+      <c r="U81" s="18"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A82" s="18"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="18"/>
+      <c r="M82" s="18"/>
+      <c r="N82" s="18"/>
+      <c r="O82" s="18"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="18"/>
+      <c r="R82" s="18"/>
+      <c r="S82" s="18"/>
+      <c r="T82" s="18"/>
+      <c r="U82" s="18"/>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A83" s="18"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="18"/>
+      <c r="O83" s="18"/>
+      <c r="P83" s="18"/>
+      <c r="Q83" s="18"/>
+      <c r="R83" s="18"/>
+      <c r="S83" s="18"/>
+      <c r="T83" s="18"/>
+      <c r="U83" s="18"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A84" s="18"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="18"/>
+      <c r="O84" s="18"/>
+      <c r="P84" s="18"/>
+      <c r="Q84" s="18"/>
+      <c r="R84" s="18"/>
+      <c r="S84" s="18"/>
+      <c r="T84" s="18"/>
+      <c r="U84" s="18"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A85" s="18"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="18"/>
+      <c r="M85" s="18"/>
+      <c r="N85" s="18"/>
+      <c r="O85" s="18"/>
+      <c r="P85" s="18"/>
+      <c r="Q85" s="18"/>
+      <c r="R85" s="18"/>
+      <c r="S85" s="18"/>
+      <c r="T85" s="18"/>
+      <c r="U85" s="18"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A86" s="18"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="18"/>
+      <c r="M86" s="18"/>
+      <c r="N86" s="18"/>
+      <c r="O86" s="18"/>
+      <c r="P86" s="18"/>
+      <c r="Q86" s="18"/>
+      <c r="R86" s="18"/>
+      <c r="S86" s="18"/>
+      <c r="T86" s="18"/>
+      <c r="U86" s="18"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A87" s="18"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
+      <c r="J87" s="18"/>
+      <c r="K87" s="18"/>
+      <c r="L87" s="18"/>
+      <c r="M87" s="18"/>
+      <c r="N87" s="18"/>
+      <c r="O87" s="18"/>
+      <c r="P87" s="18"/>
+      <c r="Q87" s="18"/>
+      <c r="R87" s="18"/>
+      <c r="S87" s="18"/>
+      <c r="T87" s="18"/>
+      <c r="U87" s="18"/>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A88" s="18"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="18"/>
+      <c r="M88" s="18"/>
+      <c r="N88" s="18"/>
+      <c r="O88" s="18"/>
+      <c r="P88" s="18"/>
+      <c r="Q88" s="18"/>
+      <c r="R88" s="18"/>
+      <c r="S88" s="18"/>
+      <c r="T88" s="18"/>
+      <c r="U88" s="18"/>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A89" s="18"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="18"/>
+      <c r="M89" s="18"/>
+      <c r="N89" s="18"/>
+      <c r="O89" s="18"/>
+      <c r="P89" s="18"/>
+      <c r="Q89" s="18"/>
+      <c r="R89" s="18"/>
+      <c r="S89" s="18"/>
+      <c r="T89" s="18"/>
+      <c r="U89" s="18"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A90" s="18"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
+      <c r="R90" s="18"/>
+      <c r="S90" s="18"/>
+      <c r="T90" s="18"/>
+      <c r="U90" s="18"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A91" s="18"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="18"/>
+      <c r="M91" s="18"/>
+      <c r="N91" s="18"/>
+      <c r="O91" s="18"/>
+      <c r="P91" s="18"/>
+      <c r="Q91" s="18"/>
+      <c r="R91" s="18"/>
+      <c r="S91" s="18"/>
+      <c r="T91" s="18"/>
+      <c r="U91" s="18"/>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A92" s="18"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="18"/>
+      <c r="M92" s="18"/>
+      <c r="N92" s="18"/>
+      <c r="O92" s="18"/>
+      <c r="P92" s="18"/>
+      <c r="Q92" s="18"/>
+      <c r="R92" s="18"/>
+      <c r="S92" s="18"/>
+      <c r="T92" s="18"/>
+      <c r="U92" s="18"/>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A93" s="18"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="18"/>
+      <c r="M93" s="18"/>
+      <c r="N93" s="18"/>
+      <c r="O93" s="18"/>
+      <c r="P93" s="18"/>
+      <c r="Q93" s="18"/>
+      <c r="R93" s="18"/>
+      <c r="S93" s="18"/>
+      <c r="T93" s="18"/>
+      <c r="U93" s="18"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A94" s="18"/>
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18"/>
+      <c r="M94" s="18"/>
+      <c r="N94" s="18"/>
+      <c r="O94" s="18"/>
+      <c r="P94" s="18"/>
+      <c r="Q94" s="18"/>
+      <c r="R94" s="18"/>
+      <c r="S94" s="18"/>
+      <c r="T94" s="18"/>
+      <c r="U94" s="18"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A95" s="18"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="18"/>
+      <c r="L95" s="18"/>
+      <c r="M95" s="18"/>
+      <c r="N95" s="18"/>
+      <c r="O95" s="18"/>
+      <c r="P95" s="18"/>
+      <c r="Q95" s="18"/>
+      <c r="R95" s="18"/>
+      <c r="S95" s="18"/>
+      <c r="T95" s="18"/>
+      <c r="U95" s="18"/>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A96" s="18"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="18"/>
+      <c r="M96" s="18"/>
+      <c r="N96" s="18"/>
+      <c r="O96" s="18"/>
+      <c r="P96" s="18"/>
+      <c r="Q96" s="18"/>
+      <c r="R96" s="18"/>
+      <c r="S96" s="18"/>
+      <c r="T96" s="18"/>
+      <c r="U96" s="18"/>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A97" s="18"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="18"/>
+      <c r="J97" s="18"/>
+      <c r="K97" s="18"/>
+      <c r="L97" s="18"/>
+      <c r="M97" s="18"/>
+      <c r="N97" s="18"/>
+      <c r="O97" s="18"/>
+      <c r="P97" s="18"/>
+      <c r="Q97" s="18"/>
+      <c r="R97" s="18"/>
+      <c r="S97" s="18"/>
+      <c r="T97" s="18"/>
+      <c r="U97" s="18"/>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A98" s="18"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="18"/>
+      <c r="J98" s="18"/>
+      <c r="K98" s="18"/>
+      <c r="L98" s="18"/>
+      <c r="M98" s="18"/>
+      <c r="N98" s="18"/>
+      <c r="O98" s="18"/>
+      <c r="P98" s="18"/>
+      <c r="Q98" s="18"/>
+      <c r="R98" s="18"/>
+      <c r="S98" s="18"/>
+      <c r="T98" s="18"/>
+      <c r="U98" s="18"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A99" s="18"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="18"/>
+      <c r="J99" s="18"/>
+      <c r="K99" s="18"/>
+      <c r="L99" s="18"/>
+      <c r="M99" s="18"/>
+      <c r="N99" s="18"/>
+      <c r="O99" s="18"/>
+      <c r="P99" s="18"/>
+      <c r="Q99" s="18"/>
+      <c r="R99" s="18"/>
+      <c r="S99" s="18"/>
+      <c r="T99" s="18"/>
+      <c r="U99" s="18"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A100" s="18"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="18"/>
+      <c r="J100" s="18"/>
+      <c r="K100" s="18"/>
+      <c r="L100" s="18"/>
+      <c r="M100" s="18"/>
+      <c r="N100" s="18"/>
+      <c r="O100" s="18"/>
+      <c r="P100" s="18"/>
+      <c r="Q100" s="18"/>
+      <c r="R100" s="18"/>
+      <c r="S100" s="18"/>
+      <c r="T100" s="18"/>
+      <c r="U100" s="18"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A101" s="18"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
+      <c r="I101" s="18"/>
+      <c r="J101" s="18"/>
+      <c r="K101" s="18"/>
+      <c r="L101" s="18"/>
+      <c r="M101" s="18"/>
+      <c r="N101" s="18"/>
+      <c r="O101" s="18"/>
+      <c r="P101" s="18"/>
+      <c r="Q101" s="18"/>
+      <c r="R101" s="18"/>
+      <c r="S101" s="18"/>
+      <c r="T101" s="18"/>
+      <c r="U101" s="18"/>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A102" s="18"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="18"/>
+      <c r="J102" s="18"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="18"/>
+      <c r="M102" s="18"/>
+      <c r="N102" s="18"/>
+      <c r="O102" s="18"/>
+      <c r="P102" s="18"/>
+      <c r="Q102" s="18"/>
+      <c r="R102" s="18"/>
+      <c r="S102" s="18"/>
+      <c r="T102" s="18"/>
+      <c r="U102" s="18"/>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A103" s="18"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="18"/>
+      <c r="M103" s="18"/>
+      <c r="N103" s="18"/>
+      <c r="O103" s="18"/>
+      <c r="P103" s="18"/>
+      <c r="Q103" s="18"/>
+      <c r="R103" s="18"/>
+      <c r="S103" s="18"/>
+      <c r="T103" s="18"/>
+      <c r="U103" s="18"/>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A104" s="18"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="18"/>
+      <c r="J104" s="18"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="18"/>
+      <c r="M104" s="18"/>
+      <c r="N104" s="18"/>
+      <c r="O104" s="18"/>
+      <c r="P104" s="18"/>
+      <c r="Q104" s="18"/>
+      <c r="R104" s="18"/>
+      <c r="S104" s="18"/>
+      <c r="T104" s="18"/>
+      <c r="U104" s="18"/>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A105" s="18"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+      <c r="K105" s="18"/>
+      <c r="L105" s="18"/>
+      <c r="M105" s="18"/>
+      <c r="N105" s="18"/>
+      <c r="O105" s="18"/>
+      <c r="P105" s="18"/>
+      <c r="Q105" s="18"/>
+      <c r="R105" s="18"/>
+      <c r="S105" s="18"/>
+      <c r="T105" s="18"/>
+      <c r="U105" s="18"/>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A106" s="18"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="18"/>
+      <c r="L106" s="18"/>
+      <c r="M106" s="18"/>
+      <c r="N106" s="18"/>
+      <c r="O106" s="18"/>
+      <c r="P106" s="18"/>
+      <c r="Q106" s="18"/>
+      <c r="R106" s="18"/>
+      <c r="S106" s="18"/>
+      <c r="T106" s="18"/>
+      <c r="U106" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="49">
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:J42"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="F30:H31"/>
     <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
     <mergeCell ref="F21:H23"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
     <mergeCell ref="F24:H26"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H17"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
+    <mergeCell ref="F18:H20"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F12:H13"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="O13:P15"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="A2:P3"/>
+    <mergeCell ref="A4:H6"/>
+    <mergeCell ref="I4:P6"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M7:P8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Avances Modulo perfil y se agrega alias a usuario
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -695,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1039,6 +1039,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4777,8 +4785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5372,14 +5380,14 @@
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
       <c r="L26" s="19"/>
-      <c r="M26" s="24" t="s">
+      <c r="M26" s="128" t="s">
         <v>80</v>
       </c>
-      <c r="N26" s="25"/>
-      <c r="O26" s="114" t="s">
+      <c r="N26" s="129"/>
+      <c r="O26" s="130" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="115"/>
+      <c r="P26" s="131"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>

</xml_diff>

<commit_message>
Creacion Sp_Address_GetAllByClient, AddressDTO, AppUserProfileDTO y mapeos
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -928,6 +928,83 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -970,12 +1047,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1030,81 +1101,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1114,8 +1116,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2471,259 +2471,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="85"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="110"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="88"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="113"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="95" t="s">
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="91"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="115"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="115"/>
+      <c r="P4" s="116"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="91"/>
+      <c r="A5" s="114"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="116"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="92"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="94"/>
+      <c r="A6" s="117"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="118"/>
+      <c r="N6" s="118"/>
+      <c r="O6" s="118"/>
+      <c r="P6" s="119"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="73" t="s">
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="105" t="s">
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="126" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="68" t="s">
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="69"/>
+      <c r="N7" s="95"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="96"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="70"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="71"/>
-      <c r="P8" s="72"/>
+      <c r="A8" s="97"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="99"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="107"/>
-      <c r="D9" s="108"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="80"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="75"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="97" t="s">
+      <c r="G9" s="102"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="122" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79" t="s">
+      <c r="J9" s="106"/>
+      <c r="K9" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="80"/>
+      <c r="L9" s="107"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="107" t="s">
+      <c r="O9" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="108"/>
+      <c r="P9" s="80"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="117"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="82"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="82"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="88"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="116" t="s">
+      <c r="O10" s="81" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="117"/>
+      <c r="P10" s="82"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="117"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="82"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="103" t="s">
+      <c r="F11" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="103"/>
-      <c r="H11" s="104"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="78"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="116" t="s">
+      <c r="K11" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="117"/>
+      <c r="L11" s="82"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="116" t="s">
+      <c r="O11" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="117"/>
+      <c r="P11" s="82"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="116"/>
-      <c r="D12" s="117"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="79" t="s">
+      <c r="F12" s="106" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="107"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="116" t="s">
+      <c r="K12" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="117"/>
+      <c r="L12" s="82"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="103" t="s">
+      <c r="O12" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="104"/>
+      <c r="P12" s="78"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -2732,23 +2732,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="88"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="116" t="s">
+      <c r="K13" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="117"/>
+      <c r="L13" s="82"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="75" t="s">
+      <c r="O13" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="76"/>
+      <c r="P13" s="103"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -2760,19 +2760,19 @@
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="103" t="s">
+      <c r="F14" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="103"/>
-      <c r="H14" s="104"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="78"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="32"/>
       <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="78"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="105"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2784,19 +2784,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="99" t="s">
+      <c r="F15" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="99"/>
-      <c r="H15" s="100"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="125"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="78"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="105"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -2806,19 +2806,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="31"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="102"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="90"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="118" t="s">
+      <c r="O16" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="119"/>
+      <c r="P16" s="72"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -2828,19 +2828,19 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="102"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="103" t="s">
+      <c r="O17" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="104"/>
+      <c r="P17" s="78"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2852,11 +2852,11 @@
       <c r="C18" s="36"/>
       <c r="D18" s="37"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="101"/>
-      <c r="H18" s="102"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="90"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -2865,10 +2865,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="120" t="s">
+      <c r="O18" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="121"/>
+      <c r="P18" s="76"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -2878,19 +2878,19 @@
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="102"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="90"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="118" t="s">
+      <c r="O19" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="119"/>
+      <c r="P19" s="72"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -2900,19 +2900,19 @@
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="102"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="90"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="118" t="s">
+      <c r="O20" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="119"/>
+      <c r="P20" s="72"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -2922,21 +2922,21 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="81" t="s">
+      <c r="F21" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="81"/>
-      <c r="H21" s="82"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="88"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="118" t="s">
+      <c r="O21" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="119"/>
+      <c r="P21" s="72"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2948,19 +2948,19 @@
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="82"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="88"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="118" t="s">
+      <c r="O22" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="119"/>
+      <c r="P22" s="72"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -2970,19 +2970,19 @@
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="82"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="88"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="124" t="s">
+      <c r="O23" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="125"/>
+      <c r="P23" s="74"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -2992,11 +2992,11 @@
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="81" t="s">
+      <c r="F24" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="81"/>
-      <c r="H24" s="82"/>
+      <c r="G24" s="91"/>
+      <c r="H24" s="88"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3005,10 +3005,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="120" t="s">
+      <c r="O24" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="121"/>
+      <c r="P24" s="76"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -3018,19 +3018,19 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="82"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="88"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="124" t="s">
+      <c r="O25" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="125"/>
+      <c r="P25" s="74"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -3042,9 +3042,9 @@
       <c r="C26" s="36"/>
       <c r="D26" s="37"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="82"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
+      <c r="H26" s="88"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -3053,10 +3053,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="25"/>
-      <c r="O26" s="122" t="s">
+      <c r="O26" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="123"/>
+      <c r="P26" s="70"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -3066,11 +3066,11 @@
       <c r="C27" s="38"/>
       <c r="D27" s="39"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="101" t="s">
+      <c r="F27" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="101"/>
-      <c r="H27" s="102"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="90"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -3079,10 +3079,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="122" t="s">
+      <c r="O27" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="123"/>
+      <c r="P27" s="70"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -3092,9 +3092,9 @@
       <c r="C28" s="38"/>
       <c r="D28" s="39"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="102"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="90"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -3103,10 +3103,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="122" t="s">
+      <c r="O28" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="123"/>
+      <c r="P28" s="70"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -3116,9 +3116,9 @@
       <c r="C29" s="38"/>
       <c r="D29" s="39"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="102"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="90"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -3127,18 +3127,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="122" t="s">
+      <c r="O29" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="123"/>
+      <c r="P29" s="70"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="81" t="s">
+      <c r="F30" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="81"/>
-      <c r="H30" s="82"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="88"/>
       <c r="L30" s="19"/>
       <c r="M30" s="23" t="s">
         <v>125</v>
@@ -3151,9 +3151,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114"/>
-      <c r="H31" s="115"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="93"/>
       <c r="L31" s="19"/>
       <c r="O31" s="30"/>
       <c r="P31" s="31"/>
@@ -3176,45 +3176,45 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="109" t="s">
+      <c r="F33" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="109"/>
-      <c r="H33" s="110"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="84"/>
       <c r="L33" s="19"/>
       <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="112"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="86"/>
       <c r="L34" s="19"/>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="112"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="86"/>
       <c r="L35" s="19"/>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="113" t="s">
+      <c r="F36" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="113"/>
-      <c r="H36" s="82"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="88"/>
       <c r="L36" s="19"/>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="113"/>
-      <c r="G37" s="113"/>
-      <c r="H37" s="82"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="88"/>
       <c r="L37" s="19"/>
       <c r="P37" s="19"/>
     </row>
@@ -4802,37 +4802,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="F30:H31"/>
     <mergeCell ref="A7:D8"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="F9:H10"/>
@@ -4849,6 +4818,37 @@
     <mergeCell ref="I7:L8"/>
     <mergeCell ref="M7:P8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4859,7 +4859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
       <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
@@ -4876,259 +4876,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="85"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="110"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="88"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="113"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="95" t="s">
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="91"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="115"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="115"/>
+      <c r="P4" s="116"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="91"/>
+      <c r="A5" s="114"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="116"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="92"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="94"/>
+      <c r="A6" s="117"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="118"/>
+      <c r="N6" s="118"/>
+      <c r="O6" s="118"/>
+      <c r="P6" s="119"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="73" t="s">
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="105" t="s">
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="126" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="68" t="s">
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="69"/>
+      <c r="N7" s="95"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="96"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="70"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="71"/>
-      <c r="P8" s="72"/>
+      <c r="A8" s="97"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="99"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="107"/>
-      <c r="D9" s="108"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="80"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="75"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="97" t="s">
+      <c r="G9" s="102"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="122" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79" t="s">
+      <c r="J9" s="106"/>
+      <c r="K9" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="80"/>
+      <c r="L9" s="107"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="107" t="s">
+      <c r="O9" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="108"/>
+      <c r="P9" s="80"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="117"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="82"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="82"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="88"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="116" t="s">
+      <c r="O10" s="81" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="117"/>
+      <c r="P10" s="82"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="117"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="82"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="103" t="s">
+      <c r="F11" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="103"/>
-      <c r="H11" s="104"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="78"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="116" t="s">
+      <c r="K11" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="117"/>
+      <c r="L11" s="82"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="116" t="s">
+      <c r="O11" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="117"/>
+      <c r="P11" s="82"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="116"/>
-      <c r="D12" s="117"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="79" t="s">
+      <c r="F12" s="106" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="107"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="116" t="s">
+      <c r="K12" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="117"/>
+      <c r="L12" s="82"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="103" t="s">
+      <c r="O12" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="104"/>
+      <c r="P12" s="78"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -5137,23 +5137,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="88"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="116" t="s">
+      <c r="K13" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="117"/>
+      <c r="L13" s="82"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="75" t="s">
+      <c r="O13" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="76"/>
+      <c r="P13" s="103"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -5165,19 +5165,19 @@
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="103" t="s">
+      <c r="F14" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="103"/>
-      <c r="H14" s="104"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="78"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="57"/>
       <c r="L14" s="58"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="78"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="105"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -5189,19 +5189,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="99" t="s">
+      <c r="F15" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="99"/>
-      <c r="H15" s="100"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="125"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="78"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="105"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -5211,19 +5211,19 @@
       <c r="C16" s="57"/>
       <c r="D16" s="58"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="102"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="90"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="118" t="s">
+      <c r="O16" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="119"/>
+      <c r="P16" s="72"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -5233,19 +5233,19 @@
       <c r="C17" s="53"/>
       <c r="D17" s="54"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="102"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="103" t="s">
+      <c r="O17" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="104"/>
+      <c r="P17" s="78"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -5257,11 +5257,11 @@
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="101"/>
-      <c r="H18" s="102"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="90"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -5270,10 +5270,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="120" t="s">
+      <c r="O18" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="121"/>
+      <c r="P18" s="76"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -5283,19 +5283,19 @@
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="102"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="90"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="118" t="s">
+      <c r="O19" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="119"/>
+      <c r="P19" s="72"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -5305,19 +5305,19 @@
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="102"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="90"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="118" t="s">
+      <c r="O20" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="119"/>
+      <c r="P20" s="72"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -5327,21 +5327,21 @@
       <c r="C21" s="49"/>
       <c r="D21" s="50"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="81" t="s">
+      <c r="F21" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="81"/>
-      <c r="H21" s="82"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="88"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="118" t="s">
+      <c r="O21" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="119"/>
+      <c r="P21" s="72"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -5353,19 +5353,19 @@
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="82"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="88"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="118" t="s">
+      <c r="O22" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="119"/>
+      <c r="P22" s="72"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -5375,19 +5375,19 @@
       <c r="C23" s="47"/>
       <c r="D23" s="48"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="82"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="88"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="124" t="s">
+      <c r="O23" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="125"/>
+      <c r="P23" s="74"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -5397,11 +5397,11 @@
       <c r="C24" s="47"/>
       <c r="D24" s="48"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="81" t="s">
+      <c r="F24" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="81"/>
-      <c r="H24" s="82"/>
+      <c r="G24" s="91"/>
+      <c r="H24" s="88"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -5410,10 +5410,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="120" t="s">
+      <c r="O24" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="121"/>
+      <c r="P24" s="76"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -5423,19 +5423,19 @@
       <c r="C25" s="49"/>
       <c r="D25" s="50"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="82"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="88"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="124" t="s">
+      <c r="O25" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="125"/>
+      <c r="P25" s="74"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -5447,17 +5447,17 @@
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="82"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
+      <c r="H26" s="88"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
       <c r="L26" s="19"/>
-      <c r="M26" s="129" t="s">
+      <c r="M26" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="N26" s="130"/>
+      <c r="N26" s="68"/>
       <c r="O26" s="131" t="s">
         <v>130</v>
       </c>
@@ -5471,11 +5471,11 @@
       <c r="C27" s="47"/>
       <c r="D27" s="48"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="101" t="s">
+      <c r="F27" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="101"/>
-      <c r="H27" s="102"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="90"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -5484,10 +5484,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="122" t="s">
+      <c r="O27" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="123"/>
+      <c r="P27" s="70"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -5497,9 +5497,9 @@
       <c r="C28" s="47"/>
       <c r="D28" s="48"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="102"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="90"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -5508,10 +5508,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="122" t="s">
+      <c r="O28" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="123"/>
+      <c r="P28" s="70"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -5521,9 +5521,9 @@
       <c r="C29" s="47"/>
       <c r="D29" s="48"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="102"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="90"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -5532,18 +5532,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="122" t="s">
+      <c r="O29" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="123"/>
+      <c r="P29" s="70"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="81" t="s">
+      <c r="F30" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="81"/>
-      <c r="H30" s="82"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="88"/>
       <c r="L30" s="19"/>
       <c r="M30" s="59" t="s">
         <v>125</v>
@@ -5557,9 +5557,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114"/>
-      <c r="H31" s="115"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="93"/>
       <c r="L31" s="19"/>
       <c r="M31" s="60"/>
       <c r="N31" s="60"/>
@@ -5587,11 +5587,11 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="109" t="s">
+      <c r="F33" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="109"/>
-      <c r="H33" s="110"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="84"/>
       <c r="L33" s="19"/>
       <c r="M33" s="60"/>
       <c r="N33" s="60"/>
@@ -5600,9 +5600,9 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="112"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="86"/>
       <c r="L34" s="19"/>
       <c r="M34" s="60"/>
       <c r="N34" s="60"/>
@@ -5611,9 +5611,9 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="112"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="86"/>
       <c r="L35" s="19"/>
       <c r="M35" s="60"/>
       <c r="N35" s="60"/>
@@ -5622,11 +5622,11 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="113" t="s">
+      <c r="F36" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="113"/>
-      <c r="H36" s="82"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="88"/>
       <c r="L36" s="19"/>
       <c r="M36" s="60"/>
       <c r="N36" s="60"/>
@@ -5635,9 +5635,9 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="113"/>
-      <c r="G37" s="113"/>
-      <c r="H37" s="82"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="88"/>
       <c r="L37" s="19"/>
       <c r="M37" s="60"/>
       <c r="N37" s="60"/>
@@ -5713,16 +5713,16 @@
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="126" t="s">
+      <c r="E41" s="128" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="127"/>
+      <c r="F41" s="129"/>
       <c r="G41" s="18"/>
-      <c r="H41" s="128" t="s">
+      <c r="H41" s="130" t="s">
         <v>132</v>
       </c>
-      <c r="I41" s="128"/>
-      <c r="J41" s="128"/>
+      <c r="I41" s="130"/>
+      <c r="J41" s="130"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
@@ -5740,12 +5740,12 @@
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="127"/>
-      <c r="F42" s="127"/>
+      <c r="E42" s="129"/>
+      <c r="F42" s="129"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="128"/>
-      <c r="I42" s="128"/>
-      <c r="J42" s="128"/>
+      <c r="H42" s="130"/>
+      <c r="I42" s="130"/>
+      <c r="J42" s="130"/>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
@@ -7232,27 +7232,20 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="H41:J42"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="A2:P3"/>
+    <mergeCell ref="A4:H6"/>
+    <mergeCell ref="I4:P6"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="K11:L11"/>
@@ -7267,20 +7260,27 @@
     <mergeCell ref="F15:H17"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="A2:P3"/>
-    <mergeCell ref="A4:H6"/>
-    <mergeCell ref="I4:P6"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:J42"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="F33:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7291,8 +7291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7346,7 +7346,7 @@
         <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finalizo modulo Mi Perfil (info, direcciones, gestion)
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -766,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -930,182 +930,188 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1116,10 +1122,29 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2471,259 +2496,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="110"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="87"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="113"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="90"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="120" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="116"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="93"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="116"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="93"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="117"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
-      <c r="N6" s="118"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="119"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="96"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="100" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="126" t="s">
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="95" t="s">
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="95"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="96"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="71"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="97"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="98"/>
-      <c r="P8" s="99"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="74"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="109" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="80"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="110"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="102" t="s">
+      <c r="F9" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="102"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="122" t="s">
+      <c r="G9" s="77"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="106"/>
-      <c r="K9" s="106" t="s">
+      <c r="J9" s="81"/>
+      <c r="K9" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="107"/>
+      <c r="L9" s="82"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="79" t="s">
+      <c r="O9" s="109" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="80"/>
+      <c r="P9" s="110"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="81"/>
-      <c r="D10" s="82"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="88"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="84"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="81" t="s">
+      <c r="O10" s="118" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="82"/>
+      <c r="P10" s="119"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="82"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="77" t="s">
+      <c r="F11" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="78"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="106"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="81" t="s">
+      <c r="K11" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="82"/>
+      <c r="L11" s="119"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="81" t="s">
+      <c r="O11" s="118" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="82"/>
+      <c r="P11" s="119"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="81"/>
-      <c r="D12" s="82"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="106" t="s">
+      <c r="F12" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="106"/>
-      <c r="H12" s="107"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="82"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="81" t="s">
+      <c r="K12" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="82"/>
+      <c r="L12" s="119"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="77" t="s">
+      <c r="O12" s="105" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="78"/>
+      <c r="P12" s="106"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -2732,23 +2757,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="88"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="84"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="81" t="s">
+      <c r="K13" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="82"/>
+      <c r="L13" s="119"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="102" t="s">
+      <c r="O13" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="103"/>
+      <c r="P13" s="78"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -2760,19 +2785,19 @@
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="78"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="106"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="32"/>
       <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="105"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="80"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2784,19 +2809,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="124" t="s">
+      <c r="F15" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="124"/>
-      <c r="H15" s="125"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="102"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="105"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="80"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -2806,19 +2831,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="31"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="90"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="71" t="s">
+      <c r="O16" s="120" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="72"/>
+      <c r="P16" s="121"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -2828,19 +2853,19 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="90"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="77" t="s">
+      <c r="O17" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="78"/>
+      <c r="P17" s="106"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2852,11 +2877,11 @@
       <c r="C18" s="36"/>
       <c r="D18" s="37"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="89" t="s">
+      <c r="F18" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="89"/>
-      <c r="H18" s="90"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="104"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -2865,10 +2890,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="75" t="s">
+      <c r="O18" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="76"/>
+      <c r="P18" s="123"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -2878,19 +2903,19 @@
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="90"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="104"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="71" t="s">
+      <c r="O19" s="120" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="72"/>
+      <c r="P19" s="121"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -2900,19 +2925,19 @@
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="90"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="104"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="71" t="s">
+      <c r="O20" s="120" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="72"/>
+      <c r="P20" s="121"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -2922,21 +2947,21 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="91" t="s">
+      <c r="F21" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="88"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="84"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="71" t="s">
+      <c r="O21" s="120" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="72"/>
+      <c r="P21" s="121"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2948,19 +2973,19 @@
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="88"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="71" t="s">
+      <c r="O22" s="120" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="72"/>
+      <c r="P22" s="121"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -2970,19 +2995,19 @@
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="88"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="84"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="73" t="s">
+      <c r="O23" s="126" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="74"/>
+      <c r="P23" s="127"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -2992,11 +3017,11 @@
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="91" t="s">
+      <c r="F24" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="91"/>
-      <c r="H24" s="88"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="84"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3005,10 +3030,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="75" t="s">
+      <c r="O24" s="122" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="76"/>
+      <c r="P24" s="123"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -3018,19 +3043,19 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="88"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="84"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="73" t="s">
+      <c r="O25" s="126" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="74"/>
+      <c r="P25" s="127"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -3042,9 +3067,9 @@
       <c r="C26" s="36"/>
       <c r="D26" s="37"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="88"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="84"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -3053,10 +3078,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="25"/>
-      <c r="O26" s="69" t="s">
+      <c r="O26" s="124" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="70"/>
+      <c r="P26" s="125"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -3066,11 +3091,11 @@
       <c r="C27" s="38"/>
       <c r="D27" s="39"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="89" t="s">
+      <c r="F27" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="89"/>
-      <c r="H27" s="90"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="104"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -3079,10 +3104,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="69" t="s">
+      <c r="O27" s="124" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="70"/>
+      <c r="P27" s="125"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -3092,9 +3117,9 @@
       <c r="C28" s="38"/>
       <c r="D28" s="39"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="90"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="104"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -3103,10 +3128,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="69" t="s">
+      <c r="O28" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="70"/>
+      <c r="P28" s="125"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -3116,9 +3141,9 @@
       <c r="C29" s="38"/>
       <c r="D29" s="39"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="90"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="104"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -3127,18 +3152,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="69" t="s">
+      <c r="O29" s="124" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="70"/>
+      <c r="P29" s="125"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="91" t="s">
+      <c r="F30" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="91"/>
-      <c r="H30" s="88"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="84"/>
       <c r="L30" s="19"/>
       <c r="M30" s="23" t="s">
         <v>125</v>
@@ -3151,9 +3176,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="93"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="117"/>
       <c r="L31" s="19"/>
       <c r="O31" s="30"/>
       <c r="P31" s="31"/>
@@ -3176,45 +3201,45 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="83" t="s">
+      <c r="F33" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="112"/>
       <c r="L33" s="19"/>
       <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="86"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="114"/>
       <c r="L34" s="19"/>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="86"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="114"/>
       <c r="L35" s="19"/>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="87" t="s">
+      <c r="F36" s="115" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="87"/>
-      <c r="H36" s="88"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="84"/>
       <c r="L36" s="19"/>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="88"/>
+      <c r="F37" s="115"/>
+      <c r="G37" s="115"/>
+      <c r="H37" s="84"/>
       <c r="L37" s="19"/>
       <c r="P37" s="19"/>
     </row>
@@ -4802,6 +4827,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="F30:H31"/>
     <mergeCell ref="A7:D8"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="F9:H10"/>
@@ -4818,37 +4874,6 @@
     <mergeCell ref="I7:L8"/>
     <mergeCell ref="M7:P8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4859,8 +4884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4876,259 +4901,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="110"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="87"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="113"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="90"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="120" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="116"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="93"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="116"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="93"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="117"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
-      <c r="N6" s="118"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="119"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="96"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="100" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="126" t="s">
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="95" t="s">
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="95"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="96"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="71"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="97"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="98"/>
-      <c r="P8" s="99"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="74"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="109" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="80"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="110"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="102" t="s">
+      <c r="F9" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="102"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="122" t="s">
+      <c r="G9" s="77"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="106"/>
-      <c r="K9" s="106" t="s">
+      <c r="J9" s="134"/>
+      <c r="K9" s="134" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="107"/>
+      <c r="L9" s="135"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="79" t="s">
+      <c r="O9" s="109" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="80"/>
+      <c r="P9" s="110"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="81"/>
-      <c r="D10" s="82"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="88"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="137"/>
+      <c r="L10" s="138"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="81" t="s">
+      <c r="O10" s="118" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="82"/>
+      <c r="P10" s="119"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="82"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="77" t="s">
+      <c r="F11" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="81" t="s">
+      <c r="G11" s="105"/>
+      <c r="H11" s="106"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="139"/>
+      <c r="K11" s="140" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="82"/>
+      <c r="L11" s="141"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="81" t="s">
+      <c r="O11" s="118" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="82"/>
+      <c r="P11" s="119"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="81"/>
-      <c r="D12" s="82"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="106" t="s">
+      <c r="F12" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="106"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="81" t="s">
+      <c r="G12" s="81"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="140" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="82"/>
+      <c r="L12" s="141"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="77" t="s">
+      <c r="O12" s="105" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="78"/>
+      <c r="P12" s="106"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -5137,23 +5162,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="81" t="s">
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="82"/>
+      <c r="L13" s="141"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="102" t="s">
+      <c r="O13" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="103"/>
+      <c r="P13" s="78"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -5165,19 +5190,19 @@
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="78"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="106"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="57"/>
       <c r="L14" s="58"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="105"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="80"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -5189,19 +5214,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="124" t="s">
+      <c r="F15" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="124"/>
-      <c r="H15" s="125"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="102"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="105"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="80"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -5211,19 +5236,19 @@
       <c r="C16" s="57"/>
       <c r="D16" s="58"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="90"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="71" t="s">
+      <c r="O16" s="120" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="72"/>
+      <c r="P16" s="121"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -5233,19 +5258,19 @@
       <c r="C17" s="53"/>
       <c r="D17" s="54"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="90"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="77" t="s">
+      <c r="O17" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="78"/>
+      <c r="P17" s="106"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -5257,11 +5282,11 @@
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="89" t="s">
+      <c r="F18" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="89"/>
-      <c r="H18" s="90"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="104"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -5270,10 +5295,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="75" t="s">
+      <c r="O18" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="76"/>
+      <c r="P18" s="123"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -5283,19 +5308,19 @@
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="90"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="104"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="71" t="s">
+      <c r="O19" s="120" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="72"/>
+      <c r="P19" s="121"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -5305,19 +5330,19 @@
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="90"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="104"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="71" t="s">
+      <c r="O20" s="120" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="72"/>
+      <c r="P20" s="121"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -5327,21 +5352,21 @@
       <c r="C21" s="49"/>
       <c r="D21" s="50"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="91" t="s">
+      <c r="F21" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="88"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="84"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="71" t="s">
+      <c r="O21" s="120" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="72"/>
+      <c r="P21" s="121"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -5353,19 +5378,19 @@
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="88"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="71" t="s">
+      <c r="O22" s="120" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="72"/>
+      <c r="P22" s="121"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -5375,19 +5400,19 @@
       <c r="C23" s="47"/>
       <c r="D23" s="48"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="88"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="84"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="73" t="s">
+      <c r="O23" s="126" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="74"/>
+      <c r="P23" s="127"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -5397,11 +5422,11 @@
       <c r="C24" s="47"/>
       <c r="D24" s="48"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="91" t="s">
+      <c r="F24" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="91"/>
-      <c r="H24" s="88"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="84"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -5410,10 +5435,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="75" t="s">
+      <c r="O24" s="122" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="76"/>
+      <c r="P24" s="123"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -5423,19 +5448,19 @@
       <c r="C25" s="49"/>
       <c r="D25" s="50"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="88"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="84"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="73" t="s">
+      <c r="O25" s="126" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="74"/>
+      <c r="P25" s="127"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -5447,9 +5472,9 @@
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="88"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="84"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -5458,10 +5483,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="68"/>
-      <c r="O26" s="131" t="s">
+      <c r="O26" s="128" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="132"/>
+      <c r="P26" s="129"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -5471,11 +5496,11 @@
       <c r="C27" s="47"/>
       <c r="D27" s="48"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="89" t="s">
+      <c r="F27" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="89"/>
-      <c r="H27" s="90"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="104"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -5484,10 +5509,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="69" t="s">
+      <c r="O27" s="124" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="70"/>
+      <c r="P27" s="125"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -5497,9 +5522,9 @@
       <c r="C28" s="47"/>
       <c r="D28" s="48"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="90"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="104"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -5508,10 +5533,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="69" t="s">
+      <c r="O28" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="70"/>
+      <c r="P28" s="125"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -5521,9 +5546,9 @@
       <c r="C29" s="47"/>
       <c r="D29" s="48"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="90"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="104"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -5532,18 +5557,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="69" t="s">
+      <c r="O29" s="124" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="70"/>
+      <c r="P29" s="125"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="91" t="s">
+      <c r="F30" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="91"/>
-      <c r="H30" s="88"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="84"/>
       <c r="L30" s="19"/>
       <c r="M30" s="59" t="s">
         <v>125</v>
@@ -5557,9 +5582,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="93"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="117"/>
       <c r="L31" s="19"/>
       <c r="M31" s="60"/>
       <c r="N31" s="60"/>
@@ -5587,11 +5612,11 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="83" t="s">
+      <c r="F33" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="112"/>
       <c r="L33" s="19"/>
       <c r="M33" s="60"/>
       <c r="N33" s="60"/>
@@ -5600,9 +5625,9 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="86"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="114"/>
       <c r="L34" s="19"/>
       <c r="M34" s="60"/>
       <c r="N34" s="60"/>
@@ -5611,9 +5636,9 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="86"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="114"/>
       <c r="L35" s="19"/>
       <c r="M35" s="60"/>
       <c r="N35" s="60"/>
@@ -5622,11 +5647,11 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="87" t="s">
+      <c r="F36" s="115" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="87"/>
-      <c r="H36" s="88"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="84"/>
       <c r="L36" s="19"/>
       <c r="M36" s="60"/>
       <c r="N36" s="60"/>
@@ -5635,9 +5660,9 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="88"/>
+      <c r="F37" s="115"/>
+      <c r="G37" s="115"/>
+      <c r="H37" s="84"/>
       <c r="L37" s="19"/>
       <c r="M37" s="60"/>
       <c r="N37" s="60"/>
@@ -5713,16 +5738,16 @@
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="128" t="s">
+      <c r="E41" s="130" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="129"/>
+      <c r="F41" s="131"/>
       <c r="G41" s="18"/>
-      <c r="H41" s="130" t="s">
+      <c r="H41" s="132" t="s">
         <v>132</v>
       </c>
-      <c r="I41" s="130"/>
-      <c r="J41" s="130"/>
+      <c r="I41" s="132"/>
+      <c r="J41" s="132"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
@@ -5740,12 +5765,12 @@
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="129"/>
-      <c r="F42" s="129"/>
+      <c r="E42" s="131"/>
+      <c r="F42" s="131"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="130"/>
-      <c r="I42" s="130"/>
-      <c r="J42" s="130"/>
+      <c r="H42" s="132"/>
+      <c r="I42" s="132"/>
+      <c r="J42" s="132"/>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
@@ -7232,20 +7257,27 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A2:P3"/>
-    <mergeCell ref="A4:H6"/>
-    <mergeCell ref="I4:P6"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:J42"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="K11:L11"/>
@@ -7260,27 +7292,20 @@
     <mergeCell ref="F15:H17"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="H41:J42"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="A2:P3"/>
+    <mergeCell ref="A4:H6"/>
+    <mergeCell ref="I4:P6"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M7:P8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7291,7 +7316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Avance Slider en Inicio
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="153">
   <si>
     <t>Nombre</t>
   </si>
@@ -480,13 +480,16 @@
   </si>
   <si>
     <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Slider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,6 +531,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -766,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -930,6 +941,82 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -972,12 +1059,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1032,80 +1113,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1113,14 +1134,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1128,25 +1146,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2496,259 +2508,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="87"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="111"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="90"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="114"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="115" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="97" t="s">
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="93"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
+      <c r="M4" s="116"/>
+      <c r="N4" s="116"/>
+      <c r="O4" s="116"/>
+      <c r="P4" s="117"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="93"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="117"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="96"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="120"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="75" t="s">
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="107" t="s">
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="127" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="70" t="s">
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="70"/>
-      <c r="O7" s="70"/>
-      <c r="P7" s="71"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="97"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="72"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="74"/>
+      <c r="A8" s="98"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="99"/>
+      <c r="N8" s="99"/>
+      <c r="O8" s="99"/>
+      <c r="P8" s="100"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="110"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="77" t="s">
+      <c r="F9" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="99" t="s">
+      <c r="G9" s="103"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="123" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81" t="s">
+      <c r="J9" s="107"/>
+      <c r="K9" s="107" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="82"/>
+      <c r="L9" s="108"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="109" t="s">
+      <c r="O9" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="110"/>
+      <c r="P9" s="81"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="118" t="s">
+      <c r="B10" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="118"/>
-      <c r="D10" s="119"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="83"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="100"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="84"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="89"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="118" t="s">
+      <c r="O10" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="119"/>
+      <c r="P10" s="83"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="119"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="105" t="s">
+      <c r="F11" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="105"/>
-      <c r="H11" s="106"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="79"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="118" t="s">
+      <c r="K11" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="119"/>
+      <c r="L11" s="83"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="118" t="s">
+      <c r="O11" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="119"/>
+      <c r="P11" s="83"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="118"/>
-      <c r="D12" s="119"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="81"/>
-      <c r="H12" s="82"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="108"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="118" t="s">
+      <c r="K12" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="119"/>
+      <c r="L12" s="83"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="105" t="s">
+      <c r="O12" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="106"/>
+      <c r="P12" s="79"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -2757,23 +2769,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="89"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="118" t="s">
+      <c r="K13" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="119"/>
+      <c r="L13" s="83"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="77" t="s">
+      <c r="O13" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="78"/>
+      <c r="P13" s="104"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -2785,19 +2797,19 @@
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="105" t="s">
+      <c r="F14" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="105"/>
-      <c r="H14" s="106"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="79"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="32"/>
       <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="80"/>
+      <c r="O14" s="105"/>
+      <c r="P14" s="106"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2809,19 +2821,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="101" t="s">
+      <c r="F15" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="101"/>
-      <c r="H15" s="102"/>
+      <c r="G15" s="125"/>
+      <c r="H15" s="126"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="80"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="106"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -2831,19 +2843,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="31"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="104"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="91"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="120" t="s">
+      <c r="O16" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="121"/>
+      <c r="P16" s="73"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -2853,19 +2865,19 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="104"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="91"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="105" t="s">
+      <c r="O17" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="106"/>
+      <c r="P17" s="79"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2877,11 +2889,11 @@
       <c r="C18" s="36"/>
       <c r="D18" s="37"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="103" t="s">
+      <c r="F18" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="103"/>
-      <c r="H18" s="104"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="91"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -2890,10 +2902,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="122" t="s">
+      <c r="O18" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="123"/>
+      <c r="P18" s="77"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -2903,19 +2915,19 @@
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="103"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="104"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="91"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="120" t="s">
+      <c r="O19" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="121"/>
+      <c r="P19" s="73"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -2925,19 +2937,19 @@
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="104"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="91"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="120" t="s">
+      <c r="O20" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="121"/>
+      <c r="P20" s="73"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -2947,21 +2959,21 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="83" t="s">
+      <c r="F21" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="83"/>
-      <c r="H21" s="84"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="89"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="120" t="s">
+      <c r="O21" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="121"/>
+      <c r="P21" s="73"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2973,19 +2985,19 @@
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="84"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="89"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="120" t="s">
+      <c r="O22" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="121"/>
+      <c r="P22" s="73"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -2995,19 +3007,19 @@
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="84"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="89"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="126" t="s">
+      <c r="O23" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="127"/>
+      <c r="P23" s="75"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -3017,11 +3029,11 @@
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="83" t="s">
+      <c r="F24" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="83"/>
-      <c r="H24" s="84"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="89"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3030,10 +3042,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="122" t="s">
+      <c r="O24" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="123"/>
+      <c r="P24" s="77"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -3043,19 +3055,19 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="84"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="89"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="126" t="s">
+      <c r="O25" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="127"/>
+      <c r="P25" s="75"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -3067,9 +3079,9 @@
       <c r="C26" s="36"/>
       <c r="D26" s="37"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="84"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="89"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -3078,10 +3090,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="25"/>
-      <c r="O26" s="124" t="s">
+      <c r="O26" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="125"/>
+      <c r="P26" s="71"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -3091,11 +3103,11 @@
       <c r="C27" s="38"/>
       <c r="D27" s="39"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="103" t="s">
+      <c r="F27" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="103"/>
-      <c r="H27" s="104"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="91"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -3104,10 +3116,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="124" t="s">
+      <c r="O27" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="125"/>
+      <c r="P27" s="71"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -3117,9 +3129,9 @@
       <c r="C28" s="38"/>
       <c r="D28" s="39"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="103"/>
-      <c r="G28" s="103"/>
-      <c r="H28" s="104"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="91"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -3128,10 +3140,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="124" t="s">
+      <c r="O28" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="125"/>
+      <c r="P28" s="71"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -3141,9 +3153,9 @@
       <c r="C29" s="38"/>
       <c r="D29" s="39"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="103"/>
-      <c r="G29" s="103"/>
-      <c r="H29" s="104"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="91"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -3152,18 +3164,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="124" t="s">
+      <c r="O29" s="70" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="125"/>
+      <c r="P29" s="71"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="83" t="s">
+      <c r="F30" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="83"/>
-      <c r="H30" s="84"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="89"/>
       <c r="L30" s="19"/>
       <c r="M30" s="23" t="s">
         <v>125</v>
@@ -3176,9 +3188,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="117"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="94"/>
       <c r="L31" s="19"/>
       <c r="O31" s="30"/>
       <c r="P31" s="31"/>
@@ -3201,45 +3213,45 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="111" t="s">
+      <c r="F33" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="111"/>
-      <c r="H33" s="112"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="85"/>
       <c r="L33" s="19"/>
       <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="113"/>
-      <c r="G34" s="113"/>
-      <c r="H34" s="114"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="87"/>
       <c r="L34" s="19"/>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="114"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="87"/>
       <c r="L35" s="19"/>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="115" t="s">
+      <c r="F36" s="88" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="115"/>
-      <c r="H36" s="84"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="89"/>
       <c r="L36" s="19"/>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="115"/>
-      <c r="G37" s="115"/>
-      <c r="H37" s="84"/>
+      <c r="F37" s="88"/>
+      <c r="G37" s="88"/>
+      <c r="H37" s="89"/>
       <c r="L37" s="19"/>
       <c r="P37" s="19"/>
     </row>
@@ -4827,37 +4839,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="F30:H31"/>
     <mergeCell ref="A7:D8"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="F9:H10"/>
@@ -4874,6 +4855,37 @@
     <mergeCell ref="I7:L8"/>
     <mergeCell ref="M7:P8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4884,8 +4896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A4" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4901,259 +4913,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="87"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="111"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="90"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="114"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="115" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="97" t="s">
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="93"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
+      <c r="M4" s="116"/>
+      <c r="N4" s="116"/>
+      <c r="O4" s="116"/>
+      <c r="P4" s="117"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="93"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="117"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="96"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="120"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="75" t="s">
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="107" t="s">
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="127" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="70" t="s">
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="70"/>
-      <c r="O7" s="70"/>
-      <c r="P7" s="71"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="97"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="72"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="74"/>
+      <c r="A8" s="98"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="99"/>
+      <c r="N8" s="99"/>
+      <c r="O8" s="99"/>
+      <c r="P8" s="100"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="110"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="77" t="s">
+      <c r="F9" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="133" t="s">
+      <c r="G9" s="103"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="136" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="134"/>
-      <c r="K9" s="134" t="s">
+      <c r="J9" s="137"/>
+      <c r="K9" s="137" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="135"/>
+      <c r="L9" s="140"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="109" t="s">
+      <c r="O9" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="110"/>
+      <c r="P9" s="81"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="118" t="s">
+      <c r="B10" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="118"/>
-      <c r="D10" s="119"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="83"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="136"/>
-      <c r="J10" s="137"/>
-      <c r="K10" s="137"/>
-      <c r="L10" s="138"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="139"/>
+      <c r="K10" s="139"/>
+      <c r="L10" s="141"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="118" t="s">
+      <c r="O10" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="119"/>
+      <c r="P10" s="83"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="119"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="105" t="s">
+      <c r="F11" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="105"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="139"/>
-      <c r="J11" s="139"/>
-      <c r="K11" s="140" t="s">
+      <c r="G11" s="78"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="134" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="141"/>
+      <c r="L11" s="135"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="118" t="s">
+      <c r="O11" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="119"/>
+      <c r="P11" s="83"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="118"/>
-      <c r="D12" s="119"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="81"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="139"/>
-      <c r="K12" s="140" t="s">
+      <c r="G12" s="107"/>
+      <c r="H12" s="108"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="134" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="141"/>
+      <c r="L12" s="135"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="105" t="s">
+      <c r="O12" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="106"/>
+      <c r="P12" s="79"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -5162,23 +5174,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="139"/>
-      <c r="J13" s="139"/>
-      <c r="K13" s="140" t="s">
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="134" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="141"/>
+      <c r="L13" s="135"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="77" t="s">
+      <c r="O13" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="78"/>
+      <c r="P13" s="104"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -5190,19 +5202,19 @@
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="105" t="s">
+      <c r="F14" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="105"/>
-      <c r="H14" s="106"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="79"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="57"/>
       <c r="L14" s="58"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="80"/>
+      <c r="O14" s="105"/>
+      <c r="P14" s="106"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -5214,19 +5226,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="101" t="s">
+      <c r="F15" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="101"/>
-      <c r="H15" s="102"/>
+      <c r="G15" s="125"/>
+      <c r="H15" s="126"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="80"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="106"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -5236,19 +5248,19 @@
       <c r="C16" s="57"/>
       <c r="D16" s="58"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="104"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="91"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="120" t="s">
+      <c r="O16" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="121"/>
+      <c r="P16" s="73"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -5258,19 +5270,19 @@
       <c r="C17" s="53"/>
       <c r="D17" s="54"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="104"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="91"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="105" t="s">
+      <c r="O17" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="106"/>
+      <c r="P17" s="79"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -5282,11 +5294,11 @@
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="103" t="s">
+      <c r="F18" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="103"/>
-      <c r="H18" s="104"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="91"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -5295,10 +5307,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="122" t="s">
+      <c r="O18" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="123"/>
+      <c r="P18" s="77"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -5308,19 +5320,19 @@
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="103"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="104"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="91"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="120" t="s">
+      <c r="O19" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="121"/>
+      <c r="P19" s="73"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -5330,19 +5342,19 @@
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="104"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="91"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="120" t="s">
+      <c r="O20" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="121"/>
+      <c r="P20" s="73"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -5352,21 +5364,21 @@
       <c r="C21" s="49"/>
       <c r="D21" s="50"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="83" t="s">
+      <c r="F21" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="83"/>
-      <c r="H21" s="84"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="89"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="120" t="s">
+      <c r="O21" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="121"/>
+      <c r="P21" s="73"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -5378,19 +5390,19 @@
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="84"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="89"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="120" t="s">
+      <c r="O22" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="121"/>
+      <c r="P22" s="73"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -5400,19 +5412,19 @@
       <c r="C23" s="47"/>
       <c r="D23" s="48"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="84"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="89"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="126" t="s">
+      <c r="O23" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="127"/>
+      <c r="P23" s="75"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -5422,11 +5434,11 @@
       <c r="C24" s="47"/>
       <c r="D24" s="48"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="83" t="s">
+      <c r="F24" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="83"/>
-      <c r="H24" s="84"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="89"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -5435,10 +5447,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="122" t="s">
+      <c r="O24" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="123"/>
+      <c r="P24" s="77"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -5448,19 +5460,19 @@
       <c r="C25" s="49"/>
       <c r="D25" s="50"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="84"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="89"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="126" t="s">
+      <c r="O25" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="127"/>
+      <c r="P25" s="75"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -5472,9 +5484,9 @@
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="84"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="89"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -5483,10 +5495,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="68"/>
-      <c r="O26" s="128" t="s">
+      <c r="O26" s="132" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="129"/>
+      <c r="P26" s="133"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -5496,11 +5508,11 @@
       <c r="C27" s="47"/>
       <c r="D27" s="48"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="103" t="s">
+      <c r="F27" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="103"/>
-      <c r="H27" s="104"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="91"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -5509,10 +5521,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="124" t="s">
+      <c r="O27" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="125"/>
+      <c r="P27" s="71"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -5522,9 +5534,9 @@
       <c r="C28" s="47"/>
       <c r="D28" s="48"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="103"/>
-      <c r="G28" s="103"/>
-      <c r="H28" s="104"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="91"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -5533,10 +5545,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="124" t="s">
+      <c r="O28" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="125"/>
+      <c r="P28" s="71"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -5546,9 +5558,9 @@
       <c r="C29" s="47"/>
       <c r="D29" s="48"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="103"/>
-      <c r="G29" s="103"/>
-      <c r="H29" s="104"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="91"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -5557,18 +5569,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="124" t="s">
+      <c r="O29" s="70" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="125"/>
+      <c r="P29" s="71"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="83" t="s">
+      <c r="F30" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="83"/>
-      <c r="H30" s="84"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="89"/>
       <c r="L30" s="19"/>
       <c r="M30" s="59" t="s">
         <v>125</v>
@@ -5582,9 +5594,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="117"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="94"/>
       <c r="L31" s="19"/>
       <c r="M31" s="60"/>
       <c r="N31" s="60"/>
@@ -5612,11 +5624,11 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="111" t="s">
+      <c r="F33" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="111"/>
-      <c r="H33" s="112"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="85"/>
       <c r="L33" s="19"/>
       <c r="M33" s="60"/>
       <c r="N33" s="60"/>
@@ -5625,9 +5637,9 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="113"/>
-      <c r="G34" s="113"/>
-      <c r="H34" s="114"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="87"/>
       <c r="L34" s="19"/>
       <c r="M34" s="60"/>
       <c r="N34" s="60"/>
@@ -5636,9 +5648,9 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="114"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="87"/>
       <c r="L35" s="19"/>
       <c r="M35" s="60"/>
       <c r="N35" s="60"/>
@@ -5647,11 +5659,11 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="115" t="s">
+      <c r="F36" s="88" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="115"/>
-      <c r="H36" s="84"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="89"/>
       <c r="L36" s="19"/>
       <c r="M36" s="60"/>
       <c r="N36" s="60"/>
@@ -5660,9 +5672,9 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="115"/>
-      <c r="G37" s="115"/>
-      <c r="H37" s="84"/>
+      <c r="F37" s="88"/>
+      <c r="G37" s="88"/>
+      <c r="H37" s="89"/>
       <c r="L37" s="19"/>
       <c r="M37" s="60"/>
       <c r="N37" s="60"/>
@@ -5738,16 +5750,16 @@
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="130" t="s">
+      <c r="E41" s="129" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="131"/>
+      <c r="F41" s="130"/>
       <c r="G41" s="18"/>
-      <c r="H41" s="132" t="s">
+      <c r="H41" s="131" t="s">
         <v>132</v>
       </c>
-      <c r="I41" s="132"/>
-      <c r="J41" s="132"/>
+      <c r="I41" s="131"/>
+      <c r="J41" s="131"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
@@ -5765,12 +5777,12 @@
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="131"/>
-      <c r="F42" s="131"/>
+      <c r="E42" s="130"/>
+      <c r="F42" s="130"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="132"/>
-      <c r="I42" s="132"/>
-      <c r="J42" s="132"/>
+      <c r="H42" s="131"/>
+      <c r="I42" s="131"/>
+      <c r="J42" s="131"/>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
@@ -7257,27 +7269,20 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="H41:J42"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="A2:P3"/>
+    <mergeCell ref="A4:H6"/>
+    <mergeCell ref="I4:P6"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="K11:L11"/>
@@ -7292,20 +7297,27 @@
     <mergeCell ref="F15:H17"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="A2:P3"/>
-    <mergeCell ref="A4:H6"/>
-    <mergeCell ref="I4:P6"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:J42"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="F33:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7314,10 +7326,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C18"/>
+  <dimension ref="B3:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7454,6 +7466,17 @@
         <v>151</v>
       </c>
     </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="142"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemento todos los repositorios faltantes
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="152">
   <si>
     <t>Nombre</t>
   </si>
@@ -477,9 +477,6 @@
   </si>
   <si>
     <t>Listo</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
   </si>
   <si>
     <t>Slider</t>
@@ -965,6 +962,87 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,12 +1085,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1067,79 +1139,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1159,39 +1189,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2542,259 +2539,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="99"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="124"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="102"/>
+      <c r="A3" s="125"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="127"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="109" t="s">
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="105"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
+      <c r="N4" s="129"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="130"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="105"/>
+      <c r="A5" s="128"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="129"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="130"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="106"/>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="107"/>
-      <c r="M6" s="107"/>
-      <c r="N6" s="107"/>
-      <c r="O6" s="107"/>
-      <c r="P6" s="108"/>
+      <c r="A6" s="131"/>
+      <c r="B6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="133"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="87" t="s">
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="119" t="s">
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="115"/>
+      <c r="I7" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="82" t="s">
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="109" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="83"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="110"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="85"/>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
-      <c r="P8" s="86"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="112"/>
+      <c r="O8" s="112"/>
+      <c r="P8" s="113"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="121" t="s">
+      <c r="B9" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="121"/>
-      <c r="D9" s="122"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="89" t="s">
+      <c r="F9" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="89"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="111" t="s">
+      <c r="G9" s="116"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="136" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="93"/>
-      <c r="K9" s="93" t="s">
+      <c r="J9" s="120"/>
+      <c r="K9" s="120" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="94"/>
+      <c r="L9" s="121"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="121" t="s">
+      <c r="O9" s="93" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="122"/>
+      <c r="P9" s="94"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="130"/>
-      <c r="D10" s="131"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="96"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="112"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="96"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="102"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="130" t="s">
+      <c r="O10" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="131"/>
+      <c r="P10" s="96"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="130"/>
-      <c r="D11" s="131"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="96"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="117"/>
-      <c r="H11" s="118"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="130" t="s">
+      <c r="K11" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="131"/>
+      <c r="L11" s="96"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="130" t="s">
+      <c r="O11" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="131"/>
+      <c r="P11" s="96"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="130"/>
-      <c r="D12" s="131"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="96"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="93" t="s">
+      <c r="F12" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="93"/>
-      <c r="H12" s="94"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="130" t="s">
+      <c r="K12" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="131"/>
+      <c r="L12" s="96"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="117" t="s">
+      <c r="O12" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="118"/>
+      <c r="P12" s="92"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -2803,23 +2800,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="96"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="102"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="130" t="s">
+      <c r="K13" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="131"/>
+      <c r="L13" s="96"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="89" t="s">
+      <c r="O13" s="116" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="90"/>
+      <c r="P13" s="117"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -2831,19 +2828,19 @@
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="117" t="s">
+      <c r="F14" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="117"/>
-      <c r="H14" s="118"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="92"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="32"/>
       <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="92"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="119"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2855,19 +2852,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="113" t="s">
+      <c r="F15" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="113"/>
-      <c r="H15" s="114"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="139"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="92"/>
+      <c r="O15" s="118"/>
+      <c r="P15" s="119"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -2877,19 +2874,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="31"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="115"/>
-      <c r="G16" s="115"/>
-      <c r="H16" s="116"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="132" t="s">
+      <c r="O16" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="133"/>
+      <c r="P16" s="86"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -2899,19 +2896,19 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="116"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="117" t="s">
+      <c r="O17" s="91" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="118"/>
+      <c r="P17" s="92"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2923,11 +2920,11 @@
       <c r="C18" s="36"/>
       <c r="D18" s="37"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="115" t="s">
+      <c r="F18" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="115"/>
-      <c r="H18" s="116"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="104"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -2936,10 +2933,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="134" t="s">
+      <c r="O18" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="135"/>
+      <c r="P18" s="90"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -2949,19 +2946,19 @@
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
-      <c r="H19" s="116"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="104"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="132" t="s">
+      <c r="O19" s="85" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="133"/>
+      <c r="P19" s="86"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -2971,19 +2968,19 @@
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="115"/>
-      <c r="H20" s="116"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="104"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="132" t="s">
+      <c r="O20" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="133"/>
+      <c r="P20" s="86"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -2993,21 +2990,21 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="95"/>
-      <c r="H21" s="96"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="102"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="132" t="s">
+      <c r="O21" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="133"/>
+      <c r="P21" s="86"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -3019,19 +3016,19 @@
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="96"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="102"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="132" t="s">
+      <c r="O22" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="133"/>
+      <c r="P22" s="86"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -3041,19 +3038,19 @@
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="96"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="102"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="138" t="s">
+      <c r="O23" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="139"/>
+      <c r="P23" s="88"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -3063,11 +3060,11 @@
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="95" t="s">
+      <c r="F24" s="105" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="95"/>
-      <c r="H24" s="96"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="102"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3076,10 +3073,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="134" t="s">
+      <c r="O24" s="89" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="135"/>
+      <c r="P24" s="90"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -3089,19 +3086,19 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="96"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="102"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="138" t="s">
+      <c r="O25" s="87" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="139"/>
+      <c r="P25" s="88"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -3113,9 +3110,9 @@
       <c r="C26" s="36"/>
       <c r="D26" s="37"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="96"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="102"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -3124,10 +3121,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="25"/>
-      <c r="O26" s="136" t="s">
+      <c r="O26" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="137"/>
+      <c r="P26" s="84"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -3137,11 +3134,11 @@
       <c r="C27" s="38"/>
       <c r="D27" s="39"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="115" t="s">
+      <c r="F27" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="115"/>
-      <c r="H27" s="116"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="104"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -3150,10 +3147,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="136" t="s">
+      <c r="O27" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="137"/>
+      <c r="P27" s="84"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -3163,9 +3160,9 @@
       <c r="C28" s="38"/>
       <c r="D28" s="39"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="116"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="104"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -3174,10 +3171,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="136" t="s">
+      <c r="O28" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="137"/>
+      <c r="P28" s="84"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -3187,9 +3184,9 @@
       <c r="C29" s="38"/>
       <c r="D29" s="39"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="116"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="104"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -3198,18 +3195,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="136" t="s">
+      <c r="O29" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="137"/>
+      <c r="P29" s="84"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="95" t="s">
+      <c r="F30" s="105" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="95"/>
-      <c r="H30" s="96"/>
+      <c r="G30" s="105"/>
+      <c r="H30" s="102"/>
       <c r="L30" s="19"/>
       <c r="M30" s="23" t="s">
         <v>125</v>
@@ -3222,9 +3219,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="128"/>
-      <c r="G31" s="128"/>
-      <c r="H31" s="129"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="107"/>
       <c r="L31" s="19"/>
       <c r="O31" s="30"/>
       <c r="P31" s="31"/>
@@ -3247,45 +3244,45 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="123" t="s">
+      <c r="F33" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="123"/>
-      <c r="H33" s="124"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="98"/>
       <c r="L33" s="19"/>
       <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="126"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
+      <c r="H34" s="100"/>
       <c r="L34" s="19"/>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="125"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="126"/>
+      <c r="F35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="100"/>
       <c r="L35" s="19"/>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="127" t="s">
+      <c r="F36" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="127"/>
-      <c r="H36" s="96"/>
+      <c r="G36" s="101"/>
+      <c r="H36" s="102"/>
       <c r="L36" s="19"/>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="127"/>
-      <c r="G37" s="127"/>
-      <c r="H37" s="96"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="102"/>
       <c r="L37" s="19"/>
       <c r="P37" s="19"/>
     </row>
@@ -4873,37 +4870,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="F30:H31"/>
     <mergeCell ref="A7:D8"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="F9:H10"/>
@@ -4920,6 +4886,37 @@
     <mergeCell ref="I7:L8"/>
     <mergeCell ref="M7:P8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4930,7 +4927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -4947,259 +4944,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="99"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="124"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="102"/>
+      <c r="A3" s="125"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="127"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="109" t="s">
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="105"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
+      <c r="N4" s="129"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="130"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="105"/>
+      <c r="A5" s="128"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="129"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="130"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="106"/>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="107"/>
-      <c r="M6" s="107"/>
-      <c r="N6" s="107"/>
-      <c r="O6" s="107"/>
-      <c r="P6" s="108"/>
+      <c r="A6" s="131"/>
+      <c r="B6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="133"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="87" t="s">
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="119" t="s">
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="115"/>
+      <c r="I7" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="82" t="s">
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="109" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="83"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="110"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="85"/>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
-      <c r="P8" s="86"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="112"/>
+      <c r="O8" s="112"/>
+      <c r="P8" s="113"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="121" t="s">
+      <c r="B9" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="121"/>
-      <c r="D9" s="122"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="89" t="s">
+      <c r="F9" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="89"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="140" t="s">
+      <c r="G9" s="116"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="151" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="141"/>
-      <c r="K9" s="141" t="s">
+      <c r="J9" s="152"/>
+      <c r="K9" s="152" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="144"/>
+      <c r="L9" s="155"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="121" t="s">
+      <c r="O9" s="93" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="122"/>
+      <c r="P9" s="94"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="130"/>
-      <c r="D10" s="131"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="96"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="142"/>
-      <c r="J10" s="143"/>
-      <c r="K10" s="143"/>
-      <c r="L10" s="145"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="153"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="154"/>
+      <c r="L10" s="156"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="130" t="s">
+      <c r="O10" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="131"/>
+      <c r="P10" s="96"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="130"/>
-      <c r="D11" s="131"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="96"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="117"/>
-      <c r="H11" s="118"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="69"/>
       <c r="J11" s="69"/>
-      <c r="K11" s="146" t="s">
+      <c r="K11" s="149" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="147"/>
+      <c r="L11" s="150"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="130" t="s">
+      <c r="O11" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="131"/>
+      <c r="P11" s="96"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="130"/>
-      <c r="D12" s="131"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="96"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="93" t="s">
+      <c r="F12" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="93"/>
-      <c r="H12" s="94"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="69"/>
       <c r="J12" s="69"/>
-      <c r="K12" s="146" t="s">
+      <c r="K12" s="149" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="147"/>
+      <c r="L12" s="150"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="117" t="s">
+      <c r="O12" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="118"/>
+      <c r="P12" s="92"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -5208,23 +5205,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="96"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="102"/>
       <c r="I13" s="69"/>
       <c r="J13" s="69"/>
-      <c r="K13" s="146" t="s">
+      <c r="K13" s="149" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="147"/>
+      <c r="L13" s="150"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="89" t="s">
+      <c r="O13" s="116" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="90"/>
+      <c r="P13" s="117"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -5236,19 +5233,19 @@
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="117" t="s">
+      <c r="F14" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="117"/>
-      <c r="H14" s="118"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="92"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="57"/>
       <c r="L14" s="58"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="92"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="119"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -5260,19 +5257,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="113" t="s">
+      <c r="F15" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="113"/>
-      <c r="H15" s="114"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="139"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="92"/>
+      <c r="O15" s="118"/>
+      <c r="P15" s="119"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -5282,19 +5279,19 @@
       <c r="C16" s="57"/>
       <c r="D16" s="58"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="115"/>
-      <c r="G16" s="115"/>
-      <c r="H16" s="116"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="132" t="s">
+      <c r="O16" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="133"/>
+      <c r="P16" s="86"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -5304,19 +5301,19 @@
       <c r="C17" s="53"/>
       <c r="D17" s="54"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="116"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="117" t="s">
+      <c r="O17" s="91" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="118"/>
+      <c r="P17" s="92"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -5328,11 +5325,11 @@
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="115" t="s">
+      <c r="F18" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="115"/>
-      <c r="H18" s="116"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="104"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -5341,10 +5338,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="23"/>
-      <c r="O18" s="155" t="s">
+      <c r="O18" s="147" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="156"/>
+      <c r="P18" s="148"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -5354,19 +5351,19 @@
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
-      <c r="H19" s="116"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="104"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="132" t="s">
+      <c r="O19" s="85" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="133"/>
+      <c r="P19" s="86"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -5376,19 +5373,19 @@
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="115"/>
-      <c r="H20" s="116"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="104"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="132" t="s">
+      <c r="O20" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="133"/>
+      <c r="P20" s="86"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -5398,21 +5395,21 @@
       <c r="C21" s="49"/>
       <c r="D21" s="50"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="95"/>
-      <c r="H21" s="96"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="102"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="132" t="s">
+      <c r="O21" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="133"/>
+      <c r="P21" s="86"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
@@ -5424,19 +5421,19 @@
       <c r="C22" s="73"/>
       <c r="D22" s="74"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="96"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="102"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="132" t="s">
+      <c r="O22" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="133"/>
+      <c r="P22" s="86"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="69"/>
@@ -5446,19 +5443,19 @@
       <c r="C23" s="79"/>
       <c r="D23" s="80"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="96"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="102"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="138" t="s">
+      <c r="O23" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="139"/>
+      <c r="P23" s="88"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="69"/>
@@ -5468,11 +5465,11 @@
       <c r="C24" s="79"/>
       <c r="D24" s="80"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="95" t="s">
+      <c r="F24" s="105" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="95"/>
-      <c r="H24" s="96"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="102"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -5481,32 +5478,32 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="134" t="s">
+      <c r="O24" s="89" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="135"/>
+      <c r="P24" s="90"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="77"/>
-      <c r="B25" s="153" t="s">
+      <c r="B25" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="153"/>
-      <c r="D25" s="154"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="82"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="96"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="102"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="138" t="s">
+      <c r="O25" s="87" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="139"/>
+      <c r="P25" s="88"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="69" t="s">
@@ -5518,9 +5515,9 @@
       <c r="C26" s="73"/>
       <c r="D26" s="74"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="96"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="102"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -5529,10 +5526,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="68"/>
-      <c r="O26" s="148" t="s">
+      <c r="O26" s="145" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="149"/>
+      <c r="P26" s="146"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="69"/>
@@ -5542,11 +5539,11 @@
       <c r="C27" s="70"/>
       <c r="D27" s="71"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="115" t="s">
+      <c r="F27" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="115"/>
-      <c r="H27" s="116"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="104"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -5555,10 +5552,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="136" t="s">
+      <c r="O27" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="137"/>
+      <c r="P27" s="84"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="69"/>
@@ -5568,9 +5565,9 @@
       <c r="C28" s="70"/>
       <c r="D28" s="71"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="116"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="104"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -5579,10 +5576,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="136" t="s">
+      <c r="O28" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="137"/>
+      <c r="P28" s="84"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="69"/>
@@ -5592,9 +5589,9 @@
       <c r="C29" s="70"/>
       <c r="D29" s="71"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="116"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="104"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -5603,21 +5600,21 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="136" t="s">
+      <c r="O29" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="137"/>
+      <c r="P29" s="84"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="75"/>
       <c r="B30" s="75"/>
       <c r="C30" s="75"/>
       <c r="D30" s="76"/>
-      <c r="F30" s="95" t="s">
+      <c r="F30" s="105" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="95"/>
-      <c r="H30" s="96"/>
+      <c r="G30" s="105"/>
+      <c r="H30" s="102"/>
       <c r="L30" s="19"/>
       <c r="M30" s="59" t="s">
         <v>125</v>
@@ -5634,9 +5631,9 @@
       <c r="C31" s="75"/>
       <c r="D31" s="76"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="128"/>
-      <c r="G31" s="128"/>
-      <c r="H31" s="129"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="107"/>
       <c r="L31" s="19"/>
       <c r="M31" s="60"/>
       <c r="N31" s="60"/>
@@ -5670,11 +5667,11 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="123" t="s">
+      <c r="F33" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="123"/>
-      <c r="H33" s="124"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="98"/>
       <c r="L33" s="19"/>
       <c r="M33" s="60"/>
       <c r="N33" s="60"/>
@@ -5686,9 +5683,9 @@
       <c r="B34" s="75"/>
       <c r="C34" s="75"/>
       <c r="D34" s="76"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="126"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
+      <c r="H34" s="100"/>
       <c r="L34" s="19"/>
       <c r="M34" s="60"/>
       <c r="N34" s="60"/>
@@ -5700,9 +5697,9 @@
       <c r="B35" s="75"/>
       <c r="C35" s="75"/>
       <c r="D35" s="76"/>
-      <c r="F35" s="125"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="126"/>
+      <c r="F35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="100"/>
       <c r="L35" s="19"/>
       <c r="M35" s="60"/>
       <c r="N35" s="60"/>
@@ -5714,11 +5711,11 @@
       <c r="B36" s="75"/>
       <c r="C36" s="75"/>
       <c r="D36" s="76"/>
-      <c r="F36" s="127" t="s">
+      <c r="F36" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="127"/>
-      <c r="H36" s="96"/>
+      <c r="G36" s="101"/>
+      <c r="H36" s="102"/>
       <c r="L36" s="19"/>
       <c r="M36" s="60"/>
       <c r="N36" s="60"/>
@@ -5730,9 +5727,9 @@
       <c r="B37" s="75"/>
       <c r="C37" s="75"/>
       <c r="D37" s="76"/>
-      <c r="F37" s="127"/>
-      <c r="G37" s="127"/>
-      <c r="H37" s="96"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="102"/>
       <c r="L37" s="19"/>
       <c r="M37" s="60"/>
       <c r="N37" s="60"/>
@@ -5808,16 +5805,16 @@
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="150" t="s">
+      <c r="E41" s="142" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="151"/>
+      <c r="F41" s="143"/>
       <c r="G41" s="18"/>
-      <c r="H41" s="152" t="s">
+      <c r="H41" s="144" t="s">
         <v>132</v>
       </c>
-      <c r="I41" s="152"/>
-      <c r="J41" s="152"/>
+      <c r="I41" s="144"/>
+      <c r="J41" s="144"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
@@ -5835,12 +5832,12 @@
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="151"/>
-      <c r="F42" s="151"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="143"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="152"/>
-      <c r="I42" s="152"/>
-      <c r="J42" s="152"/>
+      <c r="H42" s="144"/>
+      <c r="I42" s="144"/>
+      <c r="J42" s="144"/>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
@@ -7327,27 +7324,20 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="H41:J42"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="A2:P3"/>
+    <mergeCell ref="A4:H6"/>
+    <mergeCell ref="I4:P6"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="K11:L11"/>
@@ -7362,20 +7352,27 @@
     <mergeCell ref="F15:H17"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="A2:P3"/>
-    <mergeCell ref="A4:H6"/>
-    <mergeCell ref="I4:P6"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:J42"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="F33:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7386,8 +7383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7449,7 +7446,7 @@
         <v>140</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -7457,7 +7454,7 @@
         <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -7465,7 +7462,7 @@
         <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -7473,7 +7470,7 @@
         <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -7489,7 +7486,7 @@
         <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -7497,7 +7494,7 @@
         <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
@@ -7505,7 +7502,7 @@
         <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -7513,7 +7510,7 @@
         <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -7521,12 +7518,12 @@
         <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
         <v>150</v>

</xml_diff>

<commit_message>
Cambio IEnumerable por IQueryable
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -774,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -950,6 +950,84 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,12 +1070,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1052,79 +1124,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1145,72 +1211,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2560,259 +2584,259 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="121"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="96"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="98"/>
+      <c r="A3" s="122"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="124"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="105" t="s">
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="101"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="126"/>
+      <c r="N4" s="126"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="127"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="101"/>
+      <c r="A5" s="125"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="127"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="104"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
+      <c r="N6" s="129"/>
+      <c r="O6" s="129"/>
+      <c r="P6" s="130"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="83" t="s">
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="115" t="s">
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="137" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="78" t="s">
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="79"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="107"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="82"/>
+      <c r="A8" s="108"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="110"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="117" t="s">
+      <c r="B9" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="117"/>
-      <c r="D9" s="118"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="91"/>
       <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="107" t="s">
+      <c r="G9" s="113"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89" t="s">
+      <c r="J9" s="117"/>
+      <c r="K9" s="117" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="90"/>
+      <c r="L9" s="118"/>
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="18"/>
-      <c r="O9" s="117" t="s">
+      <c r="O9" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="118"/>
+      <c r="P9" s="91"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="126" t="s">
+      <c r="B10" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="126"/>
-      <c r="D10" s="127"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="93"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="92"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="116"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="99"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="126" t="s">
+      <c r="O10" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="127"/>
+      <c r="P10" s="93"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="126" t="s">
+      <c r="B11" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="126"/>
-      <c r="D11" s="127"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="93"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="113"/>
-      <c r="H11" s="114"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="89"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="126" t="s">
+      <c r="K11" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="127"/>
+      <c r="L11" s="93"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="126" t="s">
+      <c r="O11" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="127"/>
+      <c r="P11" s="93"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="126" t="s">
+      <c r="B12" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="126"/>
-      <c r="D12" s="127"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="93"/>
       <c r="E12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="89" t="s">
+      <c r="F12" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="89"/>
-      <c r="H12" s="90"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="118"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="126" t="s">
+      <c r="K12" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="127"/>
+      <c r="L12" s="93"/>
       <c r="M12" s="27"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="113" t="s">
+      <c r="O12" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="114"/>
+      <c r="P12" s="89"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
@@ -2821,23 +2845,23 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="92"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="99"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="126" t="s">
+      <c r="K13" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="127"/>
+      <c r="L13" s="93"/>
       <c r="M13" s="18" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="18"/>
-      <c r="O13" s="85" t="s">
+      <c r="O13" s="113" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="86"/>
+      <c r="P13" s="114"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -2849,19 +2873,19 @@
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="113" t="s">
+      <c r="F14" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="113"/>
-      <c r="H14" s="114"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="89"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="32"/>
       <c r="L14" s="31"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="87"/>
-      <c r="P14" s="88"/>
+      <c r="O14" s="115"/>
+      <c r="P14" s="116"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2873,19 +2897,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="109" t="s">
+      <c r="F15" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="109"/>
-      <c r="H15" s="110"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="136"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="88"/>
+      <c r="O15" s="115"/>
+      <c r="P15" s="116"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -2895,19 +2919,19 @@
       <c r="C16" s="32"/>
       <c r="D16" s="31"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="112"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="101"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="21"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="128" t="s">
+      <c r="O16" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="129"/>
+      <c r="P16" s="83"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
@@ -2917,19 +2941,19 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="112"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="101"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="113" t="s">
+      <c r="O17" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="114"/>
+      <c r="P17" s="89"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2941,11 +2965,11 @@
       <c r="C18" s="36"/>
       <c r="D18" s="37"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="111" t="s">
+      <c r="F18" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="111"/>
-      <c r="H18" s="112"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="101"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -2954,10 +2978,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="18"/>
-      <c r="O18" s="130" t="s">
+      <c r="O18" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="131"/>
+      <c r="P18" s="87"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -2967,19 +2991,19 @@
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="112"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="101"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="128" t="s">
+      <c r="O19" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="129"/>
+      <c r="P19" s="83"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -2989,19 +3013,19 @@
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="112"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="101"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="128" t="s">
+      <c r="O20" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="129"/>
+      <c r="P20" s="83"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -3011,21 +3035,21 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="91" t="s">
+      <c r="F21" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="92"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="99"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="128" t="s">
+      <c r="O21" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="129"/>
+      <c r="P21" s="83"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -3037,19 +3061,19 @@
       <c r="C22" s="36"/>
       <c r="D22" s="37"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="92"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="99"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
-      <c r="O22" s="128" t="s">
+      <c r="O22" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="129"/>
+      <c r="P22" s="83"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
@@ -3059,19 +3083,19 @@
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="92"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="99"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="27"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="134" t="s">
+      <c r="O23" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="135"/>
+      <c r="P23" s="85"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -3081,11 +3105,11 @@
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="91" t="s">
+      <c r="F24" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="91"/>
-      <c r="H24" s="92"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="99"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3094,10 +3118,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="130" t="s">
+      <c r="O24" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="131"/>
+      <c r="P24" s="87"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
@@ -3107,19 +3131,19 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="92"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="99"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="134" t="s">
+      <c r="O25" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="135"/>
+      <c r="P25" s="85"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
@@ -3131,9 +3155,9 @@
       <c r="C26" s="36"/>
       <c r="D26" s="37"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="92"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="99"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -3142,10 +3166,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="25"/>
-      <c r="O26" s="132" t="s">
+      <c r="O26" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="133"/>
+      <c r="P26" s="81"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -3155,11 +3179,11 @@
       <c r="C27" s="38"/>
       <c r="D27" s="39"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="111" t="s">
+      <c r="F27" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="111"/>
-      <c r="H27" s="112"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="101"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -3168,10 +3192,10 @@
         <v>67</v>
       </c>
       <c r="N27" s="25"/>
-      <c r="O27" s="132" t="s">
+      <c r="O27" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="133"/>
+      <c r="P27" s="81"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
@@ -3181,9 +3205,9 @@
       <c r="C28" s="38"/>
       <c r="D28" s="39"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="112"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="101"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -3192,10 +3216,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="132" t="s">
+      <c r="O28" s="80" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="133"/>
+      <c r="P28" s="81"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
@@ -3205,9 +3229,9 @@
       <c r="C29" s="38"/>
       <c r="D29" s="39"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="111"/>
-      <c r="H29" s="112"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="101"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -3216,18 +3240,18 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="132" t="s">
+      <c r="O29" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="133"/>
+      <c r="P29" s="81"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="F30" s="91" t="s">
+      <c r="F30" s="102" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="91"/>
-      <c r="H30" s="92"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="99"/>
       <c r="L30" s="19"/>
       <c r="M30" s="23" t="s">
         <v>125</v>
@@ -3240,9 +3264,9 @@
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="124"/>
-      <c r="G31" s="124"/>
-      <c r="H31" s="125"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="104"/>
       <c r="L31" s="19"/>
       <c r="O31" s="30"/>
       <c r="P31" s="31"/>
@@ -3265,45 +3289,45 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="119" t="s">
+      <c r="F33" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="119"/>
-      <c r="H33" s="120"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="95"/>
       <c r="L33" s="19"/>
       <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="122"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="97"/>
       <c r="L34" s="19"/>
       <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="122"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="97"/>
       <c r="L35" s="19"/>
       <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
-      <c r="F36" s="123" t="s">
+      <c r="F36" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="123"/>
-      <c r="H36" s="92"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="99"/>
       <c r="L36" s="19"/>
       <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="92"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="98"/>
+      <c r="H37" s="99"/>
       <c r="L37" s="19"/>
       <c r="P37" s="19"/>
     </row>
@@ -4891,37 +4915,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="F30:H31"/>
     <mergeCell ref="A7:D8"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="F9:H10"/>
@@ -4938,6 +4931,37 @@
     <mergeCell ref="I7:L8"/>
     <mergeCell ref="M7:P8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F33:H35"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4948,8 +4972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4965,260 +4989,260 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="121"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="96"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="98"/>
+      <c r="A3" s="122"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="124"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="105" t="s">
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="101"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="126"/>
+      <c r="N4" s="126"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="127"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="101"/>
+      <c r="A5" s="125"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="127"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="104"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
+      <c r="N6" s="129"/>
+      <c r="O6" s="129"/>
+      <c r="P6" s="130"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="83" t="s">
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="115" t="s">
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="137" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="78" t="s">
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="79"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="107"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="82"/>
+      <c r="A8" s="108"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="110"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="158" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="144"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="18" t="s">
+      <c r="C9" s="158"/>
+      <c r="D9" s="159"/>
+      <c r="E9" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="136" t="s">
+      <c r="G9" s="152"/>
+      <c r="H9" s="153"/>
+      <c r="I9" s="160" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="137"/>
-      <c r="K9" s="137" t="s">
+      <c r="J9" s="161"/>
+      <c r="K9" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="140"/>
+      <c r="L9" s="164"/>
       <c r="M9" s="49" t="s">
         <v>104</v>
       </c>
       <c r="N9" s="49"/>
-      <c r="O9" s="151" t="s">
+      <c r="O9" s="144" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="152"/>
+      <c r="P9" s="145"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="59"/>
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="150" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="142"/>
-      <c r="D10" s="143"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="138"/>
-      <c r="J10" s="139"/>
-      <c r="K10" s="139"/>
-      <c r="L10" s="141"/>
+      <c r="C10" s="150"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="154"/>
+      <c r="H10" s="155"/>
+      <c r="I10" s="162"/>
+      <c r="J10" s="163"/>
+      <c r="K10" s="163"/>
+      <c r="L10" s="165"/>
       <c r="M10" s="49"/>
       <c r="N10" s="49"/>
-      <c r="O10" s="153" t="s">
+      <c r="O10" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="154"/>
+      <c r="P10" s="147"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="59"/>
-      <c r="B11" s="142" t="s">
+      <c r="B11" s="150" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="142"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="113" t="s">
+      <c r="C11" s="150"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="156" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="113"/>
-      <c r="H11" s="114"/>
+      <c r="G11" s="156"/>
+      <c r="H11" s="157"/>
       <c r="I11" s="59"/>
       <c r="J11" s="59"/>
-      <c r="K11" s="142" t="s">
+      <c r="K11" s="150" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="143"/>
+      <c r="L11" s="151"/>
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
-      <c r="O11" s="153" t="s">
+      <c r="O11" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="154"/>
+      <c r="P11" s="147"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="142"/>
-      <c r="D12" s="143"/>
-      <c r="E12" s="18" t="s">
+      <c r="C12" s="150"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="89" t="s">
+      <c r="F12" s="161" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="89"/>
-      <c r="H12" s="90"/>
+      <c r="G12" s="161"/>
+      <c r="H12" s="164"/>
       <c r="I12" s="59"/>
       <c r="J12" s="59"/>
-      <c r="K12" s="142" t="s">
+      <c r="K12" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="143"/>
-      <c r="M12" s="155"/>
+      <c r="L12" s="151"/>
+      <c r="M12" s="77"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="156" t="s">
+      <c r="O12" s="148" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="157"/>
+      <c r="P12" s="149"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="67"/>
@@ -5227,24 +5251,24 @@
       </c>
       <c r="C13" s="65"/>
       <c r="D13" s="68"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="92"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="165"/>
       <c r="I13" s="59"/>
       <c r="J13" s="59"/>
-      <c r="K13" s="142" t="s">
+      <c r="K13" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="143"/>
+      <c r="L13" s="151"/>
       <c r="M13" s="59" t="s">
         <v>66</v>
       </c>
       <c r="N13" s="59"/>
-      <c r="O13" s="158" t="s">
+      <c r="O13" s="152" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="159"/>
+      <c r="P13" s="153"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="59" t="s">
@@ -5255,20 +5279,20 @@
       </c>
       <c r="C14" s="73"/>
       <c r="D14" s="74"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="113" t="s">
+      <c r="E14" s="79"/>
+      <c r="F14" s="156" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="113"/>
-      <c r="H14" s="114"/>
+      <c r="G14" s="156"/>
+      <c r="H14" s="157"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="47"/>
       <c r="L14" s="48"/>
       <c r="M14" s="59"/>
       <c r="N14" s="59"/>
-      <c r="O14" s="160"/>
-      <c r="P14" s="161"/>
+      <c r="O14" s="154"/>
+      <c r="P14" s="155"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
@@ -5280,19 +5304,19 @@
       <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="109" t="s">
+      <c r="F15" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="109"/>
-      <c r="H15" s="110"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="136"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="59"/>
       <c r="N15" s="59"/>
-      <c r="O15" s="160"/>
-      <c r="P15" s="161"/>
+      <c r="O15" s="154"/>
+      <c r="P15" s="155"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="59"/>
@@ -5302,19 +5326,19 @@
       <c r="C16" s="75"/>
       <c r="D16" s="76"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="112"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="101"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
-      <c r="M16" s="162"/>
+      <c r="M16" s="78"/>
       <c r="N16" s="59"/>
-      <c r="O16" s="142" t="s">
+      <c r="O16" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="143"/>
+      <c r="P16" s="151"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="67"/>
@@ -5324,19 +5348,19 @@
       <c r="C17" s="71"/>
       <c r="D17" s="72"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="112"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="101"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="163"/>
+      <c r="M17" s="79"/>
       <c r="N17" s="67"/>
-      <c r="O17" s="164" t="s">
+      <c r="O17" s="156" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="165"/>
+      <c r="P17" s="157"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="59" t="s">
@@ -5348,11 +5372,11 @@
       <c r="C18" s="73"/>
       <c r="D18" s="74"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="111" t="s">
+      <c r="F18" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="111"/>
-      <c r="H18" s="112"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="101"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -5361,10 +5385,10 @@
         <v>129</v>
       </c>
       <c r="N18" s="49"/>
-      <c r="O18" s="151" t="s">
+      <c r="O18" s="144" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="152"/>
+      <c r="P18" s="145"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="59"/>
@@ -5374,19 +5398,19 @@
       <c r="C19" s="75"/>
       <c r="D19" s="76"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="112"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="101"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="49"/>
       <c r="N19" s="49"/>
-      <c r="O19" s="153" t="s">
+      <c r="O19" s="146" t="s">
         <v>113</v>
       </c>
-      <c r="P19" s="154"/>
+      <c r="P19" s="147"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="59"/>
@@ -5396,19 +5420,19 @@
       <c r="C20" s="75"/>
       <c r="D20" s="76"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="112"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="101"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="49"/>
       <c r="N20" s="49"/>
-      <c r="O20" s="153" t="s">
+      <c r="O20" s="146" t="s">
         <v>114</v>
       </c>
-      <c r="P20" s="154"/>
+      <c r="P20" s="147"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67"/>
@@ -5418,21 +5442,21 @@
       <c r="C21" s="71"/>
       <c r="D21" s="72"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="91" t="s">
+      <c r="F21" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="92"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="99"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="49"/>
       <c r="N21" s="49"/>
-      <c r="O21" s="153" t="s">
+      <c r="O21" s="146" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="154"/>
+      <c r="P21" s="147"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
@@ -5444,19 +5468,19 @@
       <c r="C22" s="63"/>
       <c r="D22" s="64"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="92"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="99"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="49"/>
       <c r="N22" s="49"/>
-      <c r="O22" s="153" t="s">
+      <c r="O22" s="146" t="s">
         <v>117</v>
       </c>
-      <c r="P22" s="154"/>
+      <c r="P22" s="147"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="59"/>
@@ -5466,19 +5490,19 @@
       <c r="C23" s="69"/>
       <c r="D23" s="70"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="92"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="99"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
-      <c r="M23" s="155"/>
+      <c r="M23" s="77"/>
       <c r="N23" s="54"/>
-      <c r="O23" s="156" t="s">
+      <c r="O23" s="148" t="s">
         <v>118</v>
       </c>
-      <c r="P23" s="157"/>
+      <c r="P23" s="149"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="59"/>
@@ -5488,11 +5512,11 @@
       <c r="C24" s="69"/>
       <c r="D24" s="70"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="91" t="s">
+      <c r="F24" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="91"/>
-      <c r="H24" s="92"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="99"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -5501,10 +5525,10 @@
         <v>79</v>
       </c>
       <c r="N24" s="18"/>
-      <c r="O24" s="130" t="s">
+      <c r="O24" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="P24" s="131"/>
+      <c r="P24" s="87"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67"/>
@@ -5514,19 +5538,19 @@
       <c r="C25" s="71"/>
       <c r="D25" s="72"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="92"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="99"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="27"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="134" t="s">
+      <c r="O25" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="135"/>
+      <c r="P25" s="85"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="59" t="s">
@@ -5538,9 +5562,9 @@
       <c r="C26" s="63"/>
       <c r="D26" s="64"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="92"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="99"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
@@ -5549,10 +5573,10 @@
         <v>80</v>
       </c>
       <c r="N26" s="58"/>
-      <c r="O26" s="146" t="s">
+      <c r="O26" s="142" t="s">
         <v>130</v>
       </c>
-      <c r="P26" s="147"/>
+      <c r="P26" s="143"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="59"/>
@@ -5562,23 +5586,23 @@
       <c r="C27" s="60"/>
       <c r="D27" s="61"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="111" t="s">
+      <c r="F27" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="111"/>
-      <c r="H27" s="112"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="101"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
       <c r="L27" s="19"/>
-      <c r="M27" s="24" t="s">
+      <c r="M27" s="171" t="s">
         <v>67</v>
       </c>
-      <c r="N27" s="25"/>
-      <c r="O27" s="132" t="s">
+      <c r="N27" s="172"/>
+      <c r="O27" s="173" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="133"/>
+      <c r="P27" s="174"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="59"/>
@@ -5588,9 +5612,9 @@
       <c r="C28" s="60"/>
       <c r="D28" s="61"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="112"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="101"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -5599,10 +5623,10 @@
         <v>76</v>
       </c>
       <c r="N28" s="25"/>
-      <c r="O28" s="132" t="s">
+      <c r="O28" s="80" t="s">
         <v>123</v>
       </c>
-      <c r="P28" s="133"/>
+      <c r="P28" s="81"/>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="59"/>
@@ -5612,9 +5636,9 @@
       <c r="C29" s="60"/>
       <c r="D29" s="61"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="111"/>
-      <c r="H29" s="112"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="101"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -5623,21 +5647,21 @@
         <v>78</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="132" t="s">
+      <c r="O29" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="P29" s="133"/>
+      <c r="P29" s="81"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="65"/>
       <c r="B30" s="65"/>
       <c r="C30" s="65"/>
       <c r="D30" s="66"/>
-      <c r="F30" s="91" t="s">
+      <c r="F30" s="102" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="91"/>
-      <c r="H30" s="92"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="99"/>
       <c r="L30" s="19"/>
       <c r="M30" s="49" t="s">
         <v>125</v>
@@ -5654,9 +5678,9 @@
       <c r="C31" s="65"/>
       <c r="D31" s="66"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="124"/>
-      <c r="G31" s="124"/>
-      <c r="H31" s="125"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="104"/>
       <c r="L31" s="19"/>
       <c r="M31" s="50"/>
       <c r="N31" s="50"/>
@@ -5668,14 +5692,14 @@
       <c r="B32" s="65"/>
       <c r="C32" s="65"/>
       <c r="D32" s="66"/>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="171" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="25" t="s">
+      <c r="F32" s="172" t="s">
         <v>95</v>
       </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="26"/>
+      <c r="G32" s="172"/>
+      <c r="H32" s="175"/>
       <c r="L32" s="19"/>
       <c r="M32" s="50"/>
       <c r="N32" s="50"/>
@@ -5687,14 +5711,14 @@
       <c r="B33" s="65"/>
       <c r="C33" s="65"/>
       <c r="D33" s="66"/>
-      <c r="E33" t="s">
+      <c r="E33" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="119" t="s">
+      <c r="F33" s="166" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="119"/>
-      <c r="H33" s="120"/>
+      <c r="G33" s="166"/>
+      <c r="H33" s="167"/>
       <c r="L33" s="19"/>
       <c r="M33" s="50"/>
       <c r="N33" s="50"/>
@@ -5706,9 +5730,10 @@
       <c r="B34" s="65"/>
       <c r="C34" s="65"/>
       <c r="D34" s="66"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="122"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="168"/>
+      <c r="G34" s="168"/>
+      <c r="H34" s="169"/>
       <c r="L34" s="19"/>
       <c r="M34" s="50"/>
       <c r="N34" s="50"/>
@@ -5720,9 +5745,10 @@
       <c r="B35" s="65"/>
       <c r="C35" s="65"/>
       <c r="D35" s="66"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="122"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="168"/>
+      <c r="G35" s="168"/>
+      <c r="H35" s="169"/>
       <c r="L35" s="19"/>
       <c r="M35" s="50"/>
       <c r="N35" s="50"/>
@@ -5734,11 +5760,12 @@
       <c r="B36" s="65"/>
       <c r="C36" s="65"/>
       <c r="D36" s="66"/>
-      <c r="F36" s="123" t="s">
+      <c r="E36" s="65"/>
+      <c r="F36" s="170" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="123"/>
-      <c r="H36" s="92"/>
+      <c r="G36" s="170"/>
+      <c r="H36" s="165"/>
       <c r="L36" s="19"/>
       <c r="M36" s="50"/>
       <c r="N36" s="50"/>
@@ -5750,9 +5777,10 @@
       <c r="B37" s="65"/>
       <c r="C37" s="65"/>
       <c r="D37" s="66"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="92"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="170"/>
+      <c r="G37" s="170"/>
+      <c r="H37" s="165"/>
       <c r="L37" s="19"/>
       <c r="M37" s="50"/>
       <c r="N37" s="50"/>
@@ -5764,10 +5792,10 @@
       <c r="B38" s="67"/>
       <c r="C38" s="67"/>
       <c r="D38" s="68"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="20"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="68"/>
       <c r="I38" s="22"/>
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
@@ -5828,16 +5856,16 @@
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="148" t="s">
+      <c r="E41" s="139" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="149"/>
+      <c r="F41" s="140"/>
       <c r="G41" s="18"/>
-      <c r="H41" s="150" t="s">
+      <c r="H41" s="141" t="s">
         <v>132</v>
       </c>
-      <c r="I41" s="150"/>
-      <c r="J41" s="150"/>
+      <c r="I41" s="141"/>
+      <c r="J41" s="141"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
@@ -5855,12 +5883,12 @@
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="149"/>
-      <c r="F42" s="149"/>
+      <c r="E42" s="140"/>
+      <c r="F42" s="140"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="150"/>
-      <c r="I42" s="150"/>
-      <c r="J42" s="150"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="141"/>
+      <c r="J42" s="141"/>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
@@ -7347,27 +7375,20 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="H41:J42"/>
-    <mergeCell ref="F27:H29"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="F33:H35"/>
-    <mergeCell ref="F24:H26"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="F18:H20"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="A2:P3"/>
+    <mergeCell ref="A4:H6"/>
+    <mergeCell ref="I4:P6"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="K11:L11"/>
@@ -7382,20 +7403,27 @@
     <mergeCell ref="F15:H17"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="A2:P3"/>
-    <mergeCell ref="A4:H6"/>
-    <mergeCell ref="I4:P6"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="F18:H20"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="F24:H26"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:J42"/>
+    <mergeCell ref="F27:H29"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="F33:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>